<commit_message>
Add student and course datasets, update attendance data, and enhance Jupyter notebooks with new content and execution counts.
</commit_message>
<xml_diff>
--- a/In-class-demo/datasets/01-attendantsheet-sample.xlsx
+++ b/In-class-demo/datasets/01-attendantsheet-sample.xlsx
@@ -1,14 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="402" documentId="11_77E0E65BA4682AC65E9A93EA4535A4D85EC13015" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA04489A-38AF-4944-92BB-F50AC4A10327}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbookpro/project/tux-project/2025-System-Analysis/In-class-demo/datasets/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D143DE9-8B92-9846-9EAC-DC4FEE5573FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="21680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DevOps" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -209,8 +215,314 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={8C88BC51-6AF6-864B-B0F8-64AE69749286}</author>
+    <author>tc={30393E3D-C8F6-D644-B229-7407EF77AF94}</author>
+    <author>tc={57FD4205-72CE-084D-BC49-EC8FD345FF1D}</author>
+    <author>tc={26B80500-6755-E84E-98CA-0A974FBCE62F}</author>
+    <author>tc={F5167757-1A5A-8842-B33D-DCAEFA03BE1D}</author>
+    <author>tc={EED0A1FE-B382-9C46-A503-6F7C2FA93C99}</author>
+    <author>tc={385315BD-ADFE-8948-97FF-38612D16B638}</author>
+    <author>tc={C7512F1D-0076-DA49-96DC-6C94B0FF7368}</author>
+    <author>tc={5582C1A2-EA0E-C543-8228-EDBF0EA519AF}</author>
+    <author>tc={22C399DB-6462-F149-8055-01FBB3C6C2ED}</author>
+    <author>tc={0B524A42-E583-A14C-B114-B13A2A3DCB24}</author>
+    <author>tc={41364208-0A1F-DE41-ADE0-35101D2644AE}</author>
+    <author>tc={B964AB27-3BA4-434E-BD3C-72CC0476ABDB}</author>
+    <author>tc={90D5CF78-2AE6-8043-91E5-3D1DD7734F1C}</author>
+    <author>tc={A5883C65-A5BB-8940-B810-098C59806F74}</author>
+    <author>tc={70BFC62F-C4CA-E941-9C3B-83812FB9977A}</author>
+    <author>tc={14A5DF99-7C1B-3E47-B9F0-050C65F1B1F0}</author>
+    <author>tc={D9DD2878-73C2-4640-BC2F-B710B7C7EBE9}</author>
+    <author>tc={6F6FCFC2-8EA0-9A4F-B8D8-0F5781B4D8C8}</author>
+    <author>tc={AABB6D5C-2515-9B43-AA40-E34B761E7BB2}</author>
+    <author>tc={BE8277AD-A838-AA4B-988E-785A6734E349}</author>
+    <author>tc={E9D39B0F-2D98-AE46-909C-A2E880B360A7}</author>
+    <author>tc={0537B5AA-EB0B-F44F-9D9E-50117E078C5B}</author>
+    <author>tc={51951C8A-0B47-E84D-A952-A5BC336F732A}</author>
+    <author>tc={63AAF623-1E2E-4944-9F54-B43BCB3F82FF}</author>
+    <author>tc={815D746A-A612-4944-B652-42CA3E715E82}</author>
+    <author>tc={C949613D-92ED-2148-BC0F-0E7C1B1F31BB}</author>
+    <author>tc={755FF652-1570-1B42-9ABA-B46794BCA7E5}</author>
+    <author>tc={2F6E4008-3179-0E48-8B58-DFA7AF4C8B0A}</author>
+    <author>tc={FB8C5D10-6E1D-7E48-8E69-09F8586F80C6}</author>
+    <author>tc={FD890065-E41B-7F49-A9C1-5400C58D2DBD}</author>
+    <author>tc={1E434790-182C-964B-B40A-CF1C00311384}</author>
+    <author>tc={A9F83903-CEF2-174E-A567-64EF429A6E62}</author>
+  </authors>
+  <commentList>
+    <comment ref="B23" authorId="0" shapeId="0" xr:uid="{8C88BC51-6AF6-864B-B0F8-64AE69749286}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Reason: still working on tasks </t>
+      </text>
+    </comment>
+    <comment ref="B27" authorId="1" shapeId="0" xr:uid="{30393E3D-C8F6-D644-B229-7407EF77AF94}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    At homeland</t>
+      </text>
+    </comment>
+    <comment ref="A32" authorId="2" shapeId="0" xr:uid="{57FD4205-72CE-084D-BC49-EC8FD345FF1D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Dropped</t>
+      </text>
+    </comment>
+    <comment ref="A33" authorId="3" shapeId="0" xr:uid="{26B80500-6755-E84E-98CA-0A974FBCE62F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Dropped</t>
+      </text>
+    </comment>
+    <comment ref="A34" authorId="4" shapeId="0" xr:uid="{F5167757-1A5A-8842-B33D-DCAEFA03BE1D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Dropped</t>
+      </text>
+    </comment>
+    <comment ref="A35" authorId="5" shapeId="0" xr:uid="{EED0A1FE-B382-9C46-A503-6F7C2FA93C99}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Dropped</t>
+      </text>
+    </comment>
+    <comment ref="B35" authorId="6" shapeId="0" xr:uid="{385315BD-ADFE-8948-97FF-38612D16B638}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    student asked permission.</t>
+      </text>
+    </comment>
+    <comment ref="A36" authorId="7" shapeId="0" xr:uid="{C7512F1D-0076-DA49-96DC-6C94B0FF7368}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Dropped</t>
+      </text>
+    </comment>
+    <comment ref="A37" authorId="8" shapeId="0" xr:uid="{5582C1A2-EA0E-C543-8228-EDBF0EA519AF}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Dropped</t>
+      </text>
+    </comment>
+    <comment ref="A38" authorId="9" shapeId="0" xr:uid="{22C399DB-6462-F149-8055-01FBB3C6C2ED}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Dropped</t>
+      </text>
+    </comment>
+    <comment ref="A39" authorId="10" shapeId="0" xr:uid="{0B524A42-E583-A14C-B114-B13A2A3DCB24}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Dropped</t>
+      </text>
+    </comment>
+    <comment ref="A40" authorId="11" shapeId="0" xr:uid="{41364208-0A1F-DE41-ADE0-35101D2644AE}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Dropped</t>
+      </text>
+    </comment>
+    <comment ref="A41" authorId="12" shapeId="0" xr:uid="{B964AB27-3BA4-434E-BD3C-72CC0476ABDB}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Dropped</t>
+      </text>
+    </comment>
+    <comment ref="A42" authorId="13" shapeId="0" xr:uid="{90D5CF78-2AE6-8043-91E5-3D1DD7734F1C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Dropped</t>
+      </text>
+    </comment>
+    <comment ref="A43" authorId="14" shapeId="0" xr:uid="{A5883C65-A5BB-8940-B810-098C59806F74}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Dropped</t>
+      </text>
+    </comment>
+    <comment ref="A44" authorId="15" shapeId="0" xr:uid="{70BFC62F-C4CA-E941-9C3B-83812FB9977A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Dropped</t>
+      </text>
+    </comment>
+    <comment ref="A45" authorId="16" shapeId="0" xr:uid="{14A5DF99-7C1B-3E47-B9F0-050C65F1B1F0}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Dropped</t>
+      </text>
+    </comment>
+    <comment ref="A46" authorId="17" shapeId="0" xr:uid="{D9DD2878-73C2-4640-BC2F-B710B7C7EBE9}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Dropped</t>
+      </text>
+    </comment>
+    <comment ref="A47" authorId="18" shapeId="0" xr:uid="{6F6FCFC2-8EA0-9A4F-B8D8-0F5781B4D8C8}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Dropped</t>
+      </text>
+    </comment>
+    <comment ref="A48" authorId="19" shapeId="0" xr:uid="{AABB6D5C-2515-9B43-AA40-E34B761E7BB2}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Dropped</t>
+      </text>
+    </comment>
+    <comment ref="A49" authorId="20" shapeId="0" xr:uid="{BE8277AD-A838-AA4B-988E-785A6734E349}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Dropped</t>
+      </text>
+    </comment>
+    <comment ref="A50" authorId="21" shapeId="0" xr:uid="{E9D39B0F-2D98-AE46-909C-A2E880B360A7}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Dropped</t>
+      </text>
+    </comment>
+    <comment ref="A51" authorId="22" shapeId="0" xr:uid="{0537B5AA-EB0B-F44F-9D9E-50117E078C5B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Dropped</t>
+      </text>
+    </comment>
+    <comment ref="A52" authorId="23" shapeId="0" xr:uid="{51951C8A-0B47-E84D-A952-A5BC336F732A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Dropped</t>
+      </text>
+    </comment>
+    <comment ref="A53" authorId="24" shapeId="0" xr:uid="{63AAF623-1E2E-4944-9F54-B43BCB3F82FF}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Dropped</t>
+      </text>
+    </comment>
+    <comment ref="A54" authorId="25" shapeId="0" xr:uid="{815D746A-A612-4944-B652-42CA3E715E82}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Dropped</t>
+      </text>
+    </comment>
+    <comment ref="A55" authorId="26" shapeId="0" xr:uid="{C949613D-92ED-2148-BC0F-0E7C1B1F31BB}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Dropped</t>
+      </text>
+    </comment>
+    <comment ref="A56" authorId="27" shapeId="0" xr:uid="{755FF652-1570-1B42-9ABA-B46794BCA7E5}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Dropped</t>
+      </text>
+    </comment>
+    <comment ref="A57" authorId="28" shapeId="0" xr:uid="{2F6E4008-3179-0E48-8B58-DFA7AF4C8B0A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Dropped</t>
+      </text>
+    </comment>
+    <comment ref="A58" authorId="29" shapeId="0" xr:uid="{FB8C5D10-6E1D-7E48-8E69-09F8586F80C6}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Dropped</t>
+      </text>
+    </comment>
+    <comment ref="A59" authorId="30" shapeId="0" xr:uid="{FD890065-E41B-7F49-A9C1-5400C58D2DBD}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Dropped</t>
+      </text>
+    </comment>
+    <comment ref="A60" authorId="31" shapeId="0" xr:uid="{1E434790-182C-964B-B40A-CF1C00311384}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Dropped</t>
+      </text>
+    </comment>
+    <comment ref="A61" authorId="32" shapeId="0" xr:uid="{A9F83903-CEF2-174E-A567-64EF429A6E62}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Dropped</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="67">
   <si>
     <t>Student Attendance Sheet</t>
   </si>
@@ -512,7 +824,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -596,6 +908,12 @@
       <color rgb="FFB10202"/>
       <name val="Calibri"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -855,51 +1173,52 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="13">
     <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFFC000"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -921,6 +1240,47 @@
         <i val="0"/>
         <color rgb="FFFFC000"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFFC000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -985,9 +1345,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0529382B-C828-4B05-99A4-4D12943D3CC6}" name="Table_1" displayName="Table_1" ref="B10:B23" headerRowCount="0" headerRowDxfId="3" dataDxfId="2" totalsRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0529382B-C828-4B05-99A4-4D12943D3CC6}" name="Table_1" displayName="Table_1" ref="B10:B23" headerRowCount="0" headerRowDxfId="12" dataDxfId="11" totalsRowDxfId="10">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{1774D047-A4F4-4094-990B-C3ADC837B0CD}" name="Column1" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{1774D047-A4F4-4094-990B-C3ADC837B0CD}" name="Column1" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="Database System-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1245,6 +1605,110 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B23" dT="2025-09-06T08:50:43.21" personId="{E193429D-95C7-4F86-8233-7552E7D0E02B}" id="{8C88BC51-6AF6-864B-B0F8-64AE69749286}">
+    <text>Reason: still working on tasks </text>
+  </threadedComment>
+  <threadedComment ref="B27" dT="2025-09-27T06:26:20.01" personId="{E193429D-95C7-4F86-8233-7552E7D0E02B}" id="{30393E3D-C8F6-D644-B229-7407EF77AF94}">
+    <text>At homeland</text>
+  </threadedComment>
+  <threadedComment ref="A32" dT="2025-07-29T08:01:09.53" personId="{C26EBE42-EEB1-418C-9DAA-1751A844B8E4}" id="{57FD4205-72CE-084D-BC49-EC8FD345FF1D}">
+    <text>Dropped</text>
+  </threadedComment>
+  <threadedComment ref="A33" dT="2025-07-29T08:01:09.53" personId="{C26EBE42-EEB1-418C-9DAA-1751A844B8E4}" id="{26B80500-6755-E84E-98CA-0A974FBCE62F}">
+    <text>Dropped</text>
+  </threadedComment>
+  <threadedComment ref="A34" dT="2025-07-29T08:01:09.53" personId="{C26EBE42-EEB1-418C-9DAA-1751A844B8E4}" id="{F5167757-1A5A-8842-B33D-DCAEFA03BE1D}">
+    <text>Dropped</text>
+  </threadedComment>
+  <threadedComment ref="A35" dT="2025-07-29T08:01:09.53" personId="{C26EBE42-EEB1-418C-9DAA-1751A844B8E4}" id="{EED0A1FE-B382-9C46-A503-6F7C2FA93C99}">
+    <text>Dropped</text>
+  </threadedComment>
+  <threadedComment ref="B35" dT="2025-07-11T06:56:24.26" personId="{D148DF23-0E8B-4BDB-A073-D1BB24C69962}" id="{385315BD-ADFE-8948-97FF-38612D16B638}">
+    <text>student asked permission.</text>
+  </threadedComment>
+  <threadedComment ref="A36" dT="2025-07-29T08:01:09.53" personId="{C26EBE42-EEB1-418C-9DAA-1751A844B8E4}" id="{C7512F1D-0076-DA49-96DC-6C94B0FF7368}">
+    <text>Dropped</text>
+  </threadedComment>
+  <threadedComment ref="A37" dT="2025-07-29T08:01:09.53" personId="{C26EBE42-EEB1-418C-9DAA-1751A844B8E4}" id="{5582C1A2-EA0E-C543-8228-EDBF0EA519AF}">
+    <text>Dropped</text>
+  </threadedComment>
+  <threadedComment ref="A38" dT="2025-07-29T08:01:09.53" personId="{C26EBE42-EEB1-418C-9DAA-1751A844B8E4}" id="{22C399DB-6462-F149-8055-01FBB3C6C2ED}">
+    <text>Dropped</text>
+  </threadedComment>
+  <threadedComment ref="A39" dT="2025-07-29T08:01:09.53" personId="{C26EBE42-EEB1-418C-9DAA-1751A844B8E4}" id="{0B524A42-E583-A14C-B114-B13A2A3DCB24}">
+    <text>Dropped</text>
+  </threadedComment>
+  <threadedComment ref="A40" dT="2025-07-29T08:01:09.53" personId="{C26EBE42-EEB1-418C-9DAA-1751A844B8E4}" id="{41364208-0A1F-DE41-ADE0-35101D2644AE}">
+    <text>Dropped</text>
+  </threadedComment>
+  <threadedComment ref="A41" dT="2025-07-29T08:01:09.53" personId="{C26EBE42-EEB1-418C-9DAA-1751A844B8E4}" id="{B964AB27-3BA4-434E-BD3C-72CC0476ABDB}">
+    <text>Dropped</text>
+  </threadedComment>
+  <threadedComment ref="A42" dT="2025-07-29T08:01:09.53" personId="{C26EBE42-EEB1-418C-9DAA-1751A844B8E4}" id="{90D5CF78-2AE6-8043-91E5-3D1DD7734F1C}">
+    <text>Dropped</text>
+  </threadedComment>
+  <threadedComment ref="A43" dT="2025-07-29T08:01:09.53" personId="{C26EBE42-EEB1-418C-9DAA-1751A844B8E4}" id="{A5883C65-A5BB-8940-B810-098C59806F74}">
+    <text>Dropped</text>
+  </threadedComment>
+  <threadedComment ref="A44" dT="2025-07-29T08:01:09.53" personId="{C26EBE42-EEB1-418C-9DAA-1751A844B8E4}" id="{70BFC62F-C4CA-E941-9C3B-83812FB9977A}">
+    <text>Dropped</text>
+  </threadedComment>
+  <threadedComment ref="A45" dT="2025-07-29T08:01:09.53" personId="{C26EBE42-EEB1-418C-9DAA-1751A844B8E4}" id="{14A5DF99-7C1B-3E47-B9F0-050C65F1B1F0}">
+    <text>Dropped</text>
+  </threadedComment>
+  <threadedComment ref="A46" dT="2025-07-29T08:01:09.53" personId="{C26EBE42-EEB1-418C-9DAA-1751A844B8E4}" id="{D9DD2878-73C2-4640-BC2F-B710B7C7EBE9}">
+    <text>Dropped</text>
+  </threadedComment>
+  <threadedComment ref="A47" dT="2025-07-29T08:01:09.53" personId="{C26EBE42-EEB1-418C-9DAA-1751A844B8E4}" id="{6F6FCFC2-8EA0-9A4F-B8D8-0F5781B4D8C8}">
+    <text>Dropped</text>
+  </threadedComment>
+  <threadedComment ref="A48" dT="2025-07-29T08:01:09.53" personId="{C26EBE42-EEB1-418C-9DAA-1751A844B8E4}" id="{AABB6D5C-2515-9B43-AA40-E34B761E7BB2}">
+    <text>Dropped</text>
+  </threadedComment>
+  <threadedComment ref="A49" dT="2025-07-29T08:01:09.53" personId="{C26EBE42-EEB1-418C-9DAA-1751A844B8E4}" id="{BE8277AD-A838-AA4B-988E-785A6734E349}">
+    <text>Dropped</text>
+  </threadedComment>
+  <threadedComment ref="A50" dT="2025-07-29T08:01:09.53" personId="{C26EBE42-EEB1-418C-9DAA-1751A844B8E4}" id="{E9D39B0F-2D98-AE46-909C-A2E880B360A7}">
+    <text>Dropped</text>
+  </threadedComment>
+  <threadedComment ref="A51" dT="2025-07-29T08:01:09.53" personId="{C26EBE42-EEB1-418C-9DAA-1751A844B8E4}" id="{0537B5AA-EB0B-F44F-9D9E-50117E078C5B}">
+    <text>Dropped</text>
+  </threadedComment>
+  <threadedComment ref="A52" dT="2025-07-29T08:01:09.53" personId="{C26EBE42-EEB1-418C-9DAA-1751A844B8E4}" id="{51951C8A-0B47-E84D-A952-A5BC336F732A}">
+    <text>Dropped</text>
+  </threadedComment>
+  <threadedComment ref="A53" dT="2025-07-29T08:01:09.53" personId="{C26EBE42-EEB1-418C-9DAA-1751A844B8E4}" id="{63AAF623-1E2E-4944-9F54-B43BCB3F82FF}">
+    <text>Dropped</text>
+  </threadedComment>
+  <threadedComment ref="A54" dT="2025-07-29T08:01:09.53" personId="{C26EBE42-EEB1-418C-9DAA-1751A844B8E4}" id="{815D746A-A612-4944-B652-42CA3E715E82}">
+    <text>Dropped</text>
+  </threadedComment>
+  <threadedComment ref="A55" dT="2025-07-29T08:01:09.53" personId="{C26EBE42-EEB1-418C-9DAA-1751A844B8E4}" id="{C949613D-92ED-2148-BC0F-0E7C1B1F31BB}">
+    <text>Dropped</text>
+  </threadedComment>
+  <threadedComment ref="A56" dT="2025-07-29T08:01:09.53" personId="{C26EBE42-EEB1-418C-9DAA-1751A844B8E4}" id="{755FF652-1570-1B42-9ABA-B46794BCA7E5}">
+    <text>Dropped</text>
+  </threadedComment>
+  <threadedComment ref="A57" dT="2025-07-29T08:01:09.53" personId="{C26EBE42-EEB1-418C-9DAA-1751A844B8E4}" id="{2F6E4008-3179-0E48-8B58-DFA7AF4C8B0A}">
+    <text>Dropped</text>
+  </threadedComment>
+  <threadedComment ref="A58" dT="2025-07-29T08:01:09.53" personId="{C26EBE42-EEB1-418C-9DAA-1751A844B8E4}" id="{FB8C5D10-6E1D-7E48-8E69-09F8586F80C6}">
+    <text>Dropped</text>
+  </threadedComment>
+  <threadedComment ref="A59" dT="2025-07-29T08:01:09.53" personId="{C26EBE42-EEB1-418C-9DAA-1751A844B8E4}" id="{FD890065-E41B-7F49-A9C1-5400C58D2DBD}">
+    <text>Dropped</text>
+  </threadedComment>
+  <threadedComment ref="A60" dT="2025-07-29T08:01:09.53" personId="{C26EBE42-EEB1-418C-9DAA-1751A844B8E4}" id="{1E434790-182C-964B-B40A-CF1C00311384}">
+    <text>Dropped</text>
+  </threadedComment>
+  <threadedComment ref="A61" dT="2025-07-29T08:01:09.53" personId="{C26EBE42-EEB1-418C-9DAA-1751A844B8E4}" id="{A9F83903-CEF2-174E-A567-64EF429A6E62}">
+    <text>Dropped</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
@@ -1252,266 +1716,266 @@
   </sheetPr>
   <dimension ref="A1:AL991"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="140" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B11" sqref="B11"/>
+      <selection pane="topRight" activeCell="AH9" sqref="B9:AH23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" customWidth="1"/>
-    <col min="5" max="10" width="8.140625" customWidth="1"/>
-    <col min="11" max="38" width="6.42578125" customWidth="1"/>
+    <col min="1" max="1" width="4.5" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
+    <col min="3" max="3" width="4.6640625" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" customWidth="1"/>
+    <col min="5" max="10" width="8.1640625" customWidth="1"/>
+    <col min="11" max="38" width="6.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="14.25" customHeight="1">
+    <row r="1" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
-      <c r="Q1" s="44"/>
-      <c r="R1" s="44"/>
-      <c r="S1" s="44"/>
-      <c r="T1" s="44"/>
-      <c r="U1" s="44"/>
-      <c r="V1" s="44"/>
-      <c r="W1" s="44"/>
-      <c r="X1" s="44"/>
-      <c r="Y1" s="44"/>
-      <c r="Z1" s="44"/>
-      <c r="AA1" s="44"/>
-      <c r="AB1" s="44"/>
-      <c r="AC1" s="44"/>
-      <c r="AD1" s="44"/>
-      <c r="AE1" s="44"/>
-      <c r="AF1" s="44"/>
-      <c r="AG1" s="44"/>
-      <c r="AH1" s="44"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="40"/>
+      <c r="W1" s="40"/>
+      <c r="X1" s="40"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40"/>
+      <c r="AC1" s="40"/>
+      <c r="AD1" s="40"/>
+      <c r="AE1" s="40"/>
+      <c r="AF1" s="40"/>
+      <c r="AG1" s="40"/>
+      <c r="AH1" s="40"/>
       <c r="AI1" s="1"/>
       <c r="AJ1" s="1"/>
       <c r="AK1" s="1"/>
       <c r="AL1" s="1"/>
     </row>
-    <row r="2" spans="1:38" ht="14.25" customHeight="1">
+    <row r="2" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="44"/>
-      <c r="S2" s="44"/>
-      <c r="T2" s="44"/>
-      <c r="U2" s="44"/>
-      <c r="V2" s="44"/>
-      <c r="W2" s="44"/>
-      <c r="X2" s="44"/>
-      <c r="Y2" s="44"/>
-      <c r="Z2" s="44"/>
-      <c r="AA2" s="44"/>
-      <c r="AB2" s="44"/>
-      <c r="AC2" s="44"/>
-      <c r="AD2" s="44"/>
-      <c r="AE2" s="44"/>
-      <c r="AF2" s="44"/>
-      <c r="AG2" s="44"/>
-      <c r="AH2" s="44"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="40"/>
+      <c r="V2" s="40"/>
+      <c r="W2" s="40"/>
+      <c r="X2" s="40"/>
+      <c r="Y2" s="40"/>
+      <c r="Z2" s="40"/>
+      <c r="AA2" s="40"/>
+      <c r="AB2" s="40"/>
+      <c r="AC2" s="40"/>
+      <c r="AD2" s="40"/>
+      <c r="AE2" s="40"/>
+      <c r="AF2" s="40"/>
+      <c r="AG2" s="40"/>
+      <c r="AH2" s="40"/>
       <c r="AI2" s="1"/>
       <c r="AJ2" s="1"/>
       <c r="AK2" s="1"/>
       <c r="AL2" s="1"/>
     </row>
-    <row r="3" spans="1:38" ht="14.25" customHeight="1">
+    <row r="3" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="44"/>
-      <c r="O3" s="44"/>
-      <c r="P3" s="44"/>
-      <c r="Q3" s="44"/>
-      <c r="R3" s="44"/>
-      <c r="S3" s="44"/>
-      <c r="T3" s="44"/>
-      <c r="U3" s="44"/>
-      <c r="V3" s="44"/>
-      <c r="W3" s="44"/>
-      <c r="X3" s="44"/>
-      <c r="Y3" s="44"/>
-      <c r="Z3" s="44"/>
-      <c r="AA3" s="44"/>
-      <c r="AB3" s="44"/>
-      <c r="AC3" s="44"/>
-      <c r="AD3" s="44"/>
-      <c r="AE3" s="44"/>
-      <c r="AF3" s="44"/>
-      <c r="AG3" s="44"/>
-      <c r="AH3" s="44"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="40"/>
+      <c r="Q3" s="40"/>
+      <c r="R3" s="40"/>
+      <c r="S3" s="40"/>
+      <c r="T3" s="40"/>
+      <c r="U3" s="40"/>
+      <c r="V3" s="40"/>
+      <c r="W3" s="40"/>
+      <c r="X3" s="40"/>
+      <c r="Y3" s="40"/>
+      <c r="Z3" s="40"/>
+      <c r="AA3" s="40"/>
+      <c r="AB3" s="40"/>
+      <c r="AC3" s="40"/>
+      <c r="AD3" s="40"/>
+      <c r="AE3" s="40"/>
+      <c r="AF3" s="40"/>
+      <c r="AG3" s="40"/>
+      <c r="AH3" s="40"/>
       <c r="AI3" s="1"/>
       <c r="AJ3" s="1"/>
       <c r="AK3" s="1"/>
       <c r="AL3" s="1"/>
     </row>
-    <row r="4" spans="1:38" ht="14.25" customHeight="1">
+    <row r="4" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="44"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="44"/>
-      <c r="M4" s="44"/>
-      <c r="N4" s="44"/>
-      <c r="O4" s="44"/>
-      <c r="P4" s="44"/>
-      <c r="Q4" s="44"/>
-      <c r="R4" s="44"/>
-      <c r="S4" s="44"/>
-      <c r="T4" s="44"/>
-      <c r="U4" s="44"/>
-      <c r="V4" s="44"/>
-      <c r="W4" s="44"/>
-      <c r="X4" s="44"/>
-      <c r="Y4" s="44"/>
-      <c r="Z4" s="44"/>
-      <c r="AA4" s="44"/>
-      <c r="AB4" s="44"/>
-      <c r="AC4" s="44"/>
-      <c r="AD4" s="44"/>
-      <c r="AE4" s="44"/>
-      <c r="AF4" s="44"/>
-      <c r="AG4" s="44"/>
-      <c r="AH4" s="44"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="40"/>
+      <c r="R4" s="40"/>
+      <c r="S4" s="40"/>
+      <c r="T4" s="40"/>
+      <c r="U4" s="40"/>
+      <c r="V4" s="40"/>
+      <c r="W4" s="40"/>
+      <c r="X4" s="40"/>
+      <c r="Y4" s="40"/>
+      <c r="Z4" s="40"/>
+      <c r="AA4" s="40"/>
+      <c r="AB4" s="40"/>
+      <c r="AC4" s="40"/>
+      <c r="AD4" s="40"/>
+      <c r="AE4" s="40"/>
+      <c r="AF4" s="40"/>
+      <c r="AG4" s="40"/>
+      <c r="AH4" s="40"/>
       <c r="AI4" s="1"/>
       <c r="AJ4" s="1"/>
       <c r="AK4" s="1"/>
       <c r="AL4" s="1"/>
     </row>
-    <row r="5" spans="1:38" ht="14.25" customHeight="1">
+    <row r="5" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="44"/>
-      <c r="N5" s="44"/>
-      <c r="O5" s="44"/>
-      <c r="P5" s="44"/>
-      <c r="Q5" s="44"/>
-      <c r="R5" s="44"/>
-      <c r="S5" s="44"/>
-      <c r="T5" s="44"/>
-      <c r="U5" s="44"/>
-      <c r="V5" s="44"/>
-      <c r="W5" s="44"/>
-      <c r="X5" s="44"/>
-      <c r="Y5" s="44"/>
-      <c r="Z5" s="44"/>
-      <c r="AA5" s="44"/>
-      <c r="AB5" s="44"/>
-      <c r="AC5" s="44"/>
-      <c r="AD5" s="44"/>
-      <c r="AE5" s="44"/>
-      <c r="AF5" s="44"/>
-      <c r="AG5" s="44"/>
-      <c r="AH5" s="44"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="40"/>
+      <c r="O5" s="40"/>
+      <c r="P5" s="40"/>
+      <c r="Q5" s="40"/>
+      <c r="R5" s="40"/>
+      <c r="S5" s="40"/>
+      <c r="T5" s="40"/>
+      <c r="U5" s="40"/>
+      <c r="V5" s="40"/>
+      <c r="W5" s="40"/>
+      <c r="X5" s="40"/>
+      <c r="Y5" s="40"/>
+      <c r="Z5" s="40"/>
+      <c r="AA5" s="40"/>
+      <c r="AB5" s="40"/>
+      <c r="AC5" s="40"/>
+      <c r="AD5" s="40"/>
+      <c r="AE5" s="40"/>
+      <c r="AF5" s="40"/>
+      <c r="AG5" s="40"/>
+      <c r="AH5" s="40"/>
       <c r="AI5" s="1"/>
       <c r="AJ5" s="1"/>
       <c r="AK5" s="1"/>
       <c r="AL5" s="1"/>
     </row>
-    <row r="6" spans="1:38" ht="39.75" customHeight="1">
+    <row r="6" spans="1:38" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="39" t="s">
+      <c r="E6" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="44"/>
-      <c r="L6" s="44"/>
-      <c r="M6" s="44"/>
-      <c r="N6" s="44"/>
-      <c r="O6" s="44"/>
-      <c r="P6" s="44"/>
-      <c r="Q6" s="44"/>
-      <c r="R6" s="44"/>
-      <c r="S6" s="44"/>
-      <c r="T6" s="44"/>
-      <c r="U6" s="44"/>
-      <c r="V6" s="44"/>
-      <c r="W6" s="44"/>
-      <c r="X6" s="44"/>
-      <c r="Y6" s="44"/>
-      <c r="Z6" s="44"/>
-      <c r="AA6" s="44"/>
-      <c r="AB6" s="44"/>
-      <c r="AC6" s="44"/>
-      <c r="AD6" s="44"/>
-      <c r="AE6" s="44"/>
-      <c r="AF6" s="44"/>
-      <c r="AG6" s="44"/>
-      <c r="AH6" s="44"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="40"/>
+      <c r="Q6" s="40"/>
+      <c r="R6" s="40"/>
+      <c r="S6" s="40"/>
+      <c r="T6" s="40"/>
+      <c r="U6" s="40"/>
+      <c r="V6" s="40"/>
+      <c r="W6" s="40"/>
+      <c r="X6" s="40"/>
+      <c r="Y6" s="40"/>
+      <c r="Z6" s="40"/>
+      <c r="AA6" s="40"/>
+      <c r="AB6" s="40"/>
+      <c r="AC6" s="40"/>
+      <c r="AD6" s="40"/>
+      <c r="AE6" s="40"/>
+      <c r="AF6" s="40"/>
+      <c r="AG6" s="40"/>
+      <c r="AH6" s="40"/>
       <c r="AI6" s="2"/>
       <c r="AJ6" s="2"/>
       <c r="AK6" s="2"/>
       <c r="AL6" s="2"/>
     </row>
-    <row r="7" spans="1:38" ht="9.75" customHeight="1">
+    <row r="7" spans="1:38" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1551,13 +2015,13 @@
       <c r="AK7" s="4"/>
       <c r="AL7" s="4"/>
     </row>
-    <row r="8" spans="1:38" ht="14.25" customHeight="1">
-      <c r="A8" s="40" t="s">
+    <row r="8" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="46"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="44"/>
       <c r="E8" s="5">
         <v>45829</v>
       </c>
@@ -1648,14 +2112,14 @@
       <c r="AH8" s="5">
         <v>45941</v>
       </c>
-      <c r="AI8" s="41" t="s">
+      <c r="AI8" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="AJ8" s="45"/>
-      <c r="AK8" s="45"/>
-      <c r="AL8" s="46"/>
-    </row>
-    <row r="9" spans="1:38" ht="14.25" customHeight="1">
+      <c r="AJ8" s="43"/>
+      <c r="AK8" s="43"/>
+      <c r="AL8" s="44"/>
+    </row>
+    <row r="9" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
@@ -1771,11 +2235,11 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:38" ht="14.25" customHeight="1">
+    <row r="10" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>1</v>
       </c>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="38" t="s">
         <v>42</v>
       </c>
       <c r="C10" s="9" t="s">
@@ -1891,11 +2355,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:38" ht="14.25" customHeight="1">
+    <row r="11" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="37">
         <v>2</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="38" t="s">
         <v>45</v>
       </c>
       <c r="C11" s="9" t="s">
@@ -1963,7 +2427,7 @@
         <v>2</v>
       </c>
       <c r="AJ11" s="11">
-        <f t="shared" ref="AJ10:AJ23" si="2">COUNTIF(E11:AH11,"E")</f>
+        <f t="shared" ref="AJ11:AJ23" si="2">COUNTIF(E11:AH11,"E")</f>
         <v>2</v>
       </c>
       <c r="AK11" s="11">
@@ -1975,11 +2439,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:38" ht="14.25" customHeight="1">
+    <row r="12" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
         <v>3</v>
       </c>
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="38" t="s">
         <v>47</v>
       </c>
       <c r="C12" s="9" t="s">
@@ -2095,11 +2559,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:38" ht="14.25" customHeight="1">
+    <row r="13" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
         <v>4</v>
       </c>
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="38" t="s">
         <v>48</v>
       </c>
       <c r="C13" s="9" t="s">
@@ -2215,11 +2679,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:38" ht="14.25" customHeight="1">
+    <row r="14" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8">
         <v>5</v>
       </c>
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="38" t="s">
         <v>49</v>
       </c>
       <c r="C14" s="9" t="s">
@@ -2335,11 +2799,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:38" ht="14.25" customHeight="1">
+    <row r="15" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8">
         <v>6</v>
       </c>
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="38" t="s">
         <v>50</v>
       </c>
       <c r="C15" s="12" t="s">
@@ -2455,11 +2919,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:38" ht="14.25" customHeight="1">
+    <row r="16" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8">
         <v>7</v>
       </c>
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="38" t="s">
         <v>51</v>
       </c>
       <c r="C16" s="12" t="s">
@@ -2575,11 +3039,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:38" ht="14.25" customHeight="1">
+    <row r="17" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8">
         <v>8</v>
       </c>
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="38" t="s">
         <v>52</v>
       </c>
       <c r="C17" s="12" t="s">
@@ -2695,11 +3159,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:38" ht="14.25" customHeight="1">
+    <row r="18" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="32">
         <v>9</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="38" t="s">
         <v>53</v>
       </c>
       <c r="C18" s="30" t="s">
@@ -2811,11 +3275,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:38" ht="14.25" customHeight="1">
+    <row r="19" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="33">
         <v>10</v>
       </c>
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="38" t="s">
         <v>55</v>
       </c>
       <c r="C19" s="31" t="s">
@@ -2927,11 +3391,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:38" ht="14.25" customHeight="1">
+    <row r="20" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="33">
         <v>11</v>
       </c>
-      <c r="B20" s="43" t="s">
+      <c r="B20" s="38" t="s">
         <v>57</v>
       </c>
       <c r="C20" s="31" t="s">
@@ -3043,11 +3507,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:38" ht="14.25" customHeight="1">
+    <row r="21" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="33">
         <v>12</v>
       </c>
-      <c r="B21" s="43" t="s">
+      <c r="B21" s="38" t="s">
         <v>59</v>
       </c>
       <c r="C21" s="31" t="s">
@@ -3159,11 +3623,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:38" ht="14.25" customHeight="1">
+    <row r="22" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="33">
         <v>13</v>
       </c>
-      <c r="B22" s="43" t="s">
+      <c r="B22" s="38" t="s">
         <v>61</v>
       </c>
       <c r="C22" s="31" t="s">
@@ -3275,11 +3739,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:38" ht="14.25" customHeight="1">
+    <row r="23" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="33">
         <v>15</v>
       </c>
-      <c r="B23" s="43" t="s">
+      <c r="B23" s="38" t="s">
         <v>63</v>
       </c>
       <c r="C23" s="31" t="s">
@@ -3352,7 +3816,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:38" ht="14.25" customHeight="1">
+    <row r="24" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="8"/>
       <c r="B24" s="13"/>
       <c r="C24" s="12"/>
@@ -3392,7 +3856,7 @@
       <c r="AK24" s="11"/>
       <c r="AL24" s="11"/>
     </row>
-    <row r="25" spans="1:38" ht="14.25" customHeight="1">
+    <row r="25" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="8"/>
       <c r="B25" s="15"/>
       <c r="C25" s="12"/>
@@ -3432,54 +3896,54 @@
       <c r="AK25" s="11"/>
       <c r="AL25" s="11"/>
     </row>
-    <row r="26" spans="1:38" ht="14.25" customHeight="1">
+    <row r="26" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="16" t="s">
         <v>65</v>
       </c>
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>
       <c r="D26" s="17"/>
-      <c r="E26" s="42" t="s">
+      <c r="E26" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="F26" s="45"/>
-      <c r="G26" s="45"/>
-      <c r="H26" s="45"/>
-      <c r="I26" s="45"/>
-      <c r="J26" s="45"/>
-      <c r="K26" s="45"/>
-      <c r="L26" s="45"/>
-      <c r="M26" s="45"/>
-      <c r="N26" s="45"/>
-      <c r="O26" s="45"/>
-      <c r="P26" s="45"/>
-      <c r="Q26" s="45"/>
-      <c r="R26" s="45"/>
-      <c r="S26" s="45"/>
-      <c r="T26" s="45"/>
-      <c r="U26" s="45"/>
-      <c r="V26" s="45"/>
-      <c r="W26" s="45"/>
-      <c r="X26" s="45"/>
-      <c r="Y26" s="45"/>
-      <c r="Z26" s="45"/>
-      <c r="AA26" s="45"/>
-      <c r="AB26" s="45"/>
-      <c r="AC26" s="45"/>
-      <c r="AD26" s="45"/>
-      <c r="AE26" s="45"/>
-      <c r="AF26" s="45"/>
-      <c r="AG26" s="45"/>
-      <c r="AH26" s="45"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="43"/>
+      <c r="H26" s="43"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="43"/>
+      <c r="K26" s="43"/>
+      <c r="L26" s="43"/>
+      <c r="M26" s="43"/>
+      <c r="N26" s="43"/>
+      <c r="O26" s="43"/>
+      <c r="P26" s="43"/>
+      <c r="Q26" s="43"/>
+      <c r="R26" s="43"/>
+      <c r="S26" s="43"/>
+      <c r="T26" s="43"/>
+      <c r="U26" s="43"/>
+      <c r="V26" s="43"/>
+      <c r="W26" s="43"/>
+      <c r="X26" s="43"/>
+      <c r="Y26" s="43"/>
+      <c r="Z26" s="43"/>
+      <c r="AA26" s="43"/>
+      <c r="AB26" s="43"/>
+      <c r="AC26" s="43"/>
+      <c r="AD26" s="43"/>
+      <c r="AE26" s="43"/>
+      <c r="AF26" s="43"/>
+      <c r="AG26" s="43"/>
+      <c r="AH26" s="43"/>
       <c r="AI26" s="17"/>
       <c r="AJ26" s="17"/>
       <c r="AK26" s="17"/>
       <c r="AL26" s="18"/>
     </row>
-    <row r="27" spans="1:38" ht="6.75" customHeight="1">
+    <row r="27" spans="1:38" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D27" s="19"/>
     </row>
-    <row r="28" spans="1:38" ht="14.25" customHeight="1">
+    <row r="28" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D28" s="14" t="s">
         <v>38</v>
       </c>
@@ -3604,7 +4068,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:38" ht="14.25" customHeight="1">
+    <row r="29" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D29" s="14" t="s">
         <v>39</v>
       </c>
@@ -3729,7 +4193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:38" ht="14.25" customHeight="1">
+    <row r="30" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D30" s="14" t="s">
         <v>41</v>
       </c>
@@ -3854,967 +4318,967 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:38" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:38" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
-    <row r="49" ht="14.25" customHeight="1"/>
-    <row r="50" ht="14.25" customHeight="1"/>
-    <row r="51" ht="14.25" customHeight="1"/>
-    <row r="52" ht="14.25" customHeight="1"/>
-    <row r="53" ht="14.25" customHeight="1"/>
-    <row r="54" ht="14.25" customHeight="1"/>
-    <row r="55" ht="14.25" customHeight="1"/>
-    <row r="56" ht="14.25" customHeight="1"/>
-    <row r="57" ht="14.25" customHeight="1"/>
-    <row r="58" ht="14.25" customHeight="1"/>
-    <row r="59" ht="14.25" customHeight="1"/>
-    <row r="60" ht="14.25" customHeight="1"/>
-    <row r="61" ht="14.25" customHeight="1"/>
-    <row r="62" ht="14.25" customHeight="1"/>
-    <row r="63" ht="14.25" customHeight="1"/>
-    <row r="64" ht="14.25" customHeight="1"/>
-    <row r="65" ht="14.25" customHeight="1"/>
-    <row r="66" ht="14.25" customHeight="1"/>
-    <row r="67" ht="14.25" customHeight="1"/>
-    <row r="68" ht="14.25" customHeight="1"/>
-    <row r="69" ht="14.25" customHeight="1"/>
-    <row r="70" ht="14.25" customHeight="1"/>
-    <row r="71" ht="14.25" customHeight="1"/>
-    <row r="72" ht="14.25" customHeight="1"/>
-    <row r="73" ht="14.25" customHeight="1"/>
-    <row r="74" ht="14.25" customHeight="1"/>
-    <row r="75" ht="14.25" customHeight="1"/>
-    <row r="76" ht="14.25" customHeight="1"/>
-    <row r="77" ht="14.25" customHeight="1"/>
-    <row r="78" ht="14.25" customHeight="1"/>
-    <row r="79" ht="14.25" customHeight="1"/>
-    <row r="80" ht="14.25" customHeight="1"/>
-    <row r="81" ht="14.25" customHeight="1"/>
-    <row r="82" ht="14.25" customHeight="1"/>
-    <row r="83" ht="14.25" customHeight="1"/>
-    <row r="84" ht="14.25" customHeight="1"/>
-    <row r="85" ht="14.25" customHeight="1"/>
-    <row r="86" ht="14.25" customHeight="1"/>
-    <row r="87" ht="14.25" customHeight="1"/>
-    <row r="88" ht="14.25" customHeight="1"/>
-    <row r="89" ht="14.25" customHeight="1"/>
-    <row r="90" ht="14.25" customHeight="1"/>
-    <row r="91" ht="14.25" customHeight="1"/>
-    <row r="92" ht="14.25" customHeight="1"/>
-    <row r="93" ht="14.25" customHeight="1"/>
-    <row r="94" ht="14.25" customHeight="1"/>
-    <row r="95" ht="14.25" customHeight="1"/>
-    <row r="96" ht="14.25" customHeight="1"/>
-    <row r="97" ht="14.25" customHeight="1"/>
-    <row r="98" ht="14.25" customHeight="1"/>
-    <row r="99" ht="14.25" customHeight="1"/>
-    <row r="100" ht="14.25" customHeight="1"/>
-    <row r="101" ht="14.25" customHeight="1"/>
-    <row r="102" ht="14.25" customHeight="1"/>
-    <row r="103" ht="14.25" customHeight="1"/>
-    <row r="104" ht="14.25" customHeight="1"/>
-    <row r="105" ht="14.25" customHeight="1"/>
-    <row r="106" ht="14.25" customHeight="1"/>
-    <row r="107" ht="14.25" customHeight="1"/>
-    <row r="108" ht="14.25" customHeight="1"/>
-    <row r="109" ht="14.25" customHeight="1"/>
-    <row r="110" ht="14.25" customHeight="1"/>
-    <row r="111" ht="14.25" customHeight="1"/>
-    <row r="112" ht="14.25" customHeight="1"/>
-    <row r="113" ht="14.25" customHeight="1"/>
-    <row r="114" ht="14.25" customHeight="1"/>
-    <row r="115" ht="14.25" customHeight="1"/>
-    <row r="116" ht="14.25" customHeight="1"/>
-    <row r="117" ht="14.25" customHeight="1"/>
-    <row r="118" ht="14.25" customHeight="1"/>
-    <row r="119" ht="14.25" customHeight="1"/>
-    <row r="120" ht="14.25" customHeight="1"/>
-    <row r="121" ht="14.25" customHeight="1"/>
-    <row r="122" ht="14.25" customHeight="1"/>
-    <row r="123" ht="14.25" customHeight="1"/>
-    <row r="124" ht="14.25" customHeight="1"/>
-    <row r="125" ht="14.25" customHeight="1"/>
-    <row r="126" ht="14.25" customHeight="1"/>
-    <row r="127" ht="14.25" customHeight="1"/>
-    <row r="128" ht="14.25" customHeight="1"/>
-    <row r="129" ht="14.25" customHeight="1"/>
-    <row r="130" ht="14.25" customHeight="1"/>
-    <row r="131" ht="14.25" customHeight="1"/>
-    <row r="132" ht="14.25" customHeight="1"/>
-    <row r="133" ht="14.25" customHeight="1"/>
-    <row r="134" ht="14.25" customHeight="1"/>
-    <row r="135" ht="14.25" customHeight="1"/>
-    <row r="136" ht="14.25" customHeight="1"/>
-    <row r="137" ht="14.25" customHeight="1"/>
-    <row r="138" ht="14.25" customHeight="1"/>
-    <row r="139" ht="14.25" customHeight="1"/>
-    <row r="140" ht="14.25" customHeight="1"/>
-    <row r="141" ht="14.25" customHeight="1"/>
-    <row r="142" ht="14.25" customHeight="1"/>
-    <row r="143" ht="14.25" customHeight="1"/>
-    <row r="144" ht="14.25" customHeight="1"/>
-    <row r="145" ht="14.25" customHeight="1"/>
-    <row r="146" ht="14.25" customHeight="1"/>
-    <row r="147" ht="14.25" customHeight="1"/>
-    <row r="148" ht="14.25" customHeight="1"/>
-    <row r="149" ht="14.25" customHeight="1"/>
-    <row r="150" ht="14.25" customHeight="1"/>
-    <row r="151" ht="14.25" customHeight="1"/>
-    <row r="152" ht="14.25" customHeight="1"/>
-    <row r="153" ht="14.25" customHeight="1"/>
-    <row r="154" ht="14.25" customHeight="1"/>
-    <row r="155" ht="14.25" customHeight="1"/>
-    <row r="156" ht="14.25" customHeight="1"/>
-    <row r="157" ht="14.25" customHeight="1"/>
-    <row r="158" ht="14.25" customHeight="1"/>
-    <row r="159" ht="14.25" customHeight="1"/>
-    <row r="160" ht="14.25" customHeight="1"/>
-    <row r="161" ht="14.25" customHeight="1"/>
-    <row r="162" ht="14.25" customHeight="1"/>
-    <row r="163" ht="14.25" customHeight="1"/>
-    <row r="164" ht="14.25" customHeight="1"/>
-    <row r="165" ht="14.25" customHeight="1"/>
-    <row r="166" ht="14.25" customHeight="1"/>
-    <row r="167" ht="14.25" customHeight="1"/>
-    <row r="168" ht="14.25" customHeight="1"/>
-    <row r="169" ht="14.25" customHeight="1"/>
-    <row r="170" ht="14.25" customHeight="1"/>
-    <row r="171" ht="14.25" customHeight="1"/>
-    <row r="172" ht="14.25" customHeight="1"/>
-    <row r="173" ht="14.25" customHeight="1"/>
-    <row r="174" ht="14.25" customHeight="1"/>
-    <row r="175" ht="14.25" customHeight="1"/>
-    <row r="176" ht="14.25" customHeight="1"/>
-    <row r="177" ht="14.25" customHeight="1"/>
-    <row r="178" ht="14.25" customHeight="1"/>
-    <row r="179" ht="14.25" customHeight="1"/>
-    <row r="180" ht="14.25" customHeight="1"/>
-    <row r="181" ht="14.25" customHeight="1"/>
-    <row r="182" ht="14.25" customHeight="1"/>
-    <row r="183" ht="14.25" customHeight="1"/>
-    <row r="184" ht="14.25" customHeight="1"/>
-    <row r="185" ht="14.25" customHeight="1"/>
-    <row r="186" ht="14.25" customHeight="1"/>
-    <row r="187" ht="14.25" customHeight="1"/>
-    <row r="188" ht="14.25" customHeight="1"/>
-    <row r="189" ht="14.25" customHeight="1"/>
-    <row r="190" ht="14.25" customHeight="1"/>
-    <row r="191" ht="14.25" customHeight="1"/>
-    <row r="192" ht="14.25" customHeight="1"/>
-    <row r="193" ht="14.25" customHeight="1"/>
-    <row r="194" ht="14.25" customHeight="1"/>
-    <row r="195" ht="14.25" customHeight="1"/>
-    <row r="196" ht="14.25" customHeight="1"/>
-    <row r="197" ht="14.25" customHeight="1"/>
-    <row r="198" ht="14.25" customHeight="1"/>
-    <row r="199" ht="14.25" customHeight="1"/>
-    <row r="200" ht="14.25" customHeight="1"/>
-    <row r="201" ht="14.25" customHeight="1"/>
-    <row r="202" ht="14.25" customHeight="1"/>
-    <row r="203" ht="14.25" customHeight="1"/>
-    <row r="204" ht="14.25" customHeight="1"/>
-    <row r="205" ht="14.25" customHeight="1"/>
-    <row r="206" ht="14.25" customHeight="1"/>
-    <row r="207" ht="14.25" customHeight="1"/>
-    <row r="208" ht="14.25" customHeight="1"/>
-    <row r="209" ht="14.25" customHeight="1"/>
-    <row r="210" ht="14.25" customHeight="1"/>
-    <row r="211" ht="14.25" customHeight="1"/>
-    <row r="212" ht="14.25" customHeight="1"/>
-    <row r="213" ht="14.25" customHeight="1"/>
-    <row r="214" ht="14.25" customHeight="1"/>
-    <row r="215" ht="14.25" customHeight="1"/>
-    <row r="216" ht="14.25" customHeight="1"/>
-    <row r="217" ht="14.25" customHeight="1"/>
-    <row r="218" ht="14.25" customHeight="1"/>
-    <row r="219" ht="14.25" customHeight="1"/>
-    <row r="220" ht="14.25" customHeight="1"/>
-    <row r="221" ht="14.25" customHeight="1"/>
-    <row r="222" ht="14.25" customHeight="1"/>
-    <row r="223" ht="14.25" customHeight="1"/>
-    <row r="224" ht="14.25" customHeight="1"/>
-    <row r="225" ht="14.25" customHeight="1"/>
-    <row r="226" ht="14.25" customHeight="1"/>
-    <row r="227" ht="14.25" customHeight="1"/>
-    <row r="228" ht="14.25" customHeight="1"/>
-    <row r="229" ht="14.25" customHeight="1"/>
-    <row r="230" ht="14.25" customHeight="1"/>
-    <row r="231" ht="14.25" customHeight="1"/>
-    <row r="232" ht="14.25" customHeight="1"/>
-    <row r="233" ht="14.25" customHeight="1"/>
-    <row r="234" ht="14.25" customHeight="1"/>
-    <row r="235" ht="14.25" customHeight="1"/>
-    <row r="236" ht="14.25" customHeight="1"/>
-    <row r="237" ht="14.25" customHeight="1"/>
-    <row r="238" ht="14.25" customHeight="1"/>
-    <row r="239" ht="14.25" customHeight="1"/>
-    <row r="240" ht="14.25" customHeight="1"/>
-    <row r="241" ht="14.25" customHeight="1"/>
-    <row r="242" ht="14.25" customHeight="1"/>
-    <row r="243" ht="14.25" customHeight="1"/>
-    <row r="244" ht="14.25" customHeight="1"/>
-    <row r="245" ht="14.25" customHeight="1"/>
-    <row r="246" ht="14.25" customHeight="1"/>
-    <row r="247" ht="14.25" customHeight="1"/>
-    <row r="248" ht="14.25" customHeight="1"/>
-    <row r="249" ht="14.25" customHeight="1"/>
-    <row r="250" ht="14.25" customHeight="1"/>
-    <row r="251" ht="14.25" customHeight="1"/>
-    <row r="252" ht="14.25" customHeight="1"/>
-    <row r="253" ht="14.25" customHeight="1"/>
-    <row r="254" ht="14.25" customHeight="1"/>
-    <row r="255" ht="14.25" customHeight="1"/>
-    <row r="256" ht="14.25" customHeight="1"/>
-    <row r="257" ht="14.25" customHeight="1"/>
-    <row r="258" ht="14.25" customHeight="1"/>
-    <row r="259" ht="14.25" customHeight="1"/>
-    <row r="260" ht="14.25" customHeight="1"/>
-    <row r="261" ht="14.25" customHeight="1"/>
-    <row r="262" ht="14.25" customHeight="1"/>
-    <row r="263" ht="14.25" customHeight="1"/>
-    <row r="264" ht="14.25" customHeight="1"/>
-    <row r="265" ht="14.25" customHeight="1"/>
-    <row r="266" ht="14.25" customHeight="1"/>
-    <row r="267" ht="14.25" customHeight="1"/>
-    <row r="268" ht="14.25" customHeight="1"/>
-    <row r="269" ht="14.25" customHeight="1"/>
-    <row r="270" ht="14.25" customHeight="1"/>
-    <row r="271" ht="14.25" customHeight="1"/>
-    <row r="272" ht="14.25" customHeight="1"/>
-    <row r="273" ht="14.25" customHeight="1"/>
-    <row r="274" ht="14.25" customHeight="1"/>
-    <row r="275" ht="14.25" customHeight="1"/>
-    <row r="276" ht="14.25" customHeight="1"/>
-    <row r="277" ht="14.25" customHeight="1"/>
-    <row r="278" ht="14.25" customHeight="1"/>
-    <row r="279" ht="14.25" customHeight="1"/>
-    <row r="280" ht="14.25" customHeight="1"/>
-    <row r="281" ht="14.25" customHeight="1"/>
-    <row r="282" ht="14.25" customHeight="1"/>
-    <row r="283" ht="14.25" customHeight="1"/>
-    <row r="284" ht="14.25" customHeight="1"/>
-    <row r="285" ht="14.25" customHeight="1"/>
-    <row r="286" ht="14.25" customHeight="1"/>
-    <row r="287" ht="14.25" customHeight="1"/>
-    <row r="288" ht="14.25" customHeight="1"/>
-    <row r="289" ht="14.25" customHeight="1"/>
-    <row r="290" ht="14.25" customHeight="1"/>
-    <row r="291" ht="14.25" customHeight="1"/>
-    <row r="292" ht="14.25" customHeight="1"/>
-    <row r="293" ht="14.25" customHeight="1"/>
-    <row r="294" ht="14.25" customHeight="1"/>
-    <row r="295" ht="14.25" customHeight="1"/>
-    <row r="296" ht="14.25" customHeight="1"/>
-    <row r="297" ht="14.25" customHeight="1"/>
-    <row r="298" ht="14.25" customHeight="1"/>
-    <row r="299" ht="14.25" customHeight="1"/>
-    <row r="300" ht="14.25" customHeight="1"/>
-    <row r="301" ht="14.25" customHeight="1"/>
-    <row r="302" ht="14.25" customHeight="1"/>
-    <row r="303" ht="14.25" customHeight="1"/>
-    <row r="304" ht="14.25" customHeight="1"/>
-    <row r="305" ht="14.25" customHeight="1"/>
-    <row r="306" ht="14.25" customHeight="1"/>
-    <row r="307" ht="14.25" customHeight="1"/>
-    <row r="308" ht="14.25" customHeight="1"/>
-    <row r="309" ht="14.25" customHeight="1"/>
-    <row r="310" ht="14.25" customHeight="1"/>
-    <row r="311" ht="14.25" customHeight="1"/>
-    <row r="312" ht="14.25" customHeight="1"/>
-    <row r="313" ht="14.25" customHeight="1"/>
-    <row r="314" ht="14.25" customHeight="1"/>
-    <row r="315" ht="14.25" customHeight="1"/>
-    <row r="316" ht="14.25" customHeight="1"/>
-    <row r="317" ht="14.25" customHeight="1"/>
-    <row r="318" ht="14.25" customHeight="1"/>
-    <row r="319" ht="14.25" customHeight="1"/>
-    <row r="320" ht="14.25" customHeight="1"/>
-    <row r="321" ht="14.25" customHeight="1"/>
-    <row r="322" ht="14.25" customHeight="1"/>
-    <row r="323" ht="14.25" customHeight="1"/>
-    <row r="324" ht="14.25" customHeight="1"/>
-    <row r="325" ht="14.25" customHeight="1"/>
-    <row r="326" ht="14.25" customHeight="1"/>
-    <row r="327" ht="14.25" customHeight="1"/>
-    <row r="328" ht="14.25" customHeight="1"/>
-    <row r="329" ht="14.25" customHeight="1"/>
-    <row r="330" ht="14.25" customHeight="1"/>
-    <row r="331" ht="14.25" customHeight="1"/>
-    <row r="332" ht="14.25" customHeight="1"/>
-    <row r="333" ht="14.25" customHeight="1"/>
-    <row r="334" ht="14.25" customHeight="1"/>
-    <row r="335" ht="14.25" customHeight="1"/>
-    <row r="336" ht="14.25" customHeight="1"/>
-    <row r="337" ht="14.25" customHeight="1"/>
-    <row r="338" ht="14.25" customHeight="1"/>
-    <row r="339" ht="14.25" customHeight="1"/>
-    <row r="340" ht="14.25" customHeight="1"/>
-    <row r="341" ht="14.25" customHeight="1"/>
-    <row r="342" ht="14.25" customHeight="1"/>
-    <row r="343" ht="14.25" customHeight="1"/>
-    <row r="344" ht="14.25" customHeight="1"/>
-    <row r="345" ht="14.25" customHeight="1"/>
-    <row r="346" ht="14.25" customHeight="1"/>
-    <row r="347" ht="14.25" customHeight="1"/>
-    <row r="348" ht="14.25" customHeight="1"/>
-    <row r="349" ht="14.25" customHeight="1"/>
-    <row r="350" ht="14.25" customHeight="1"/>
-    <row r="351" ht="14.25" customHeight="1"/>
-    <row r="352" ht="14.25" customHeight="1"/>
-    <row r="353" ht="14.25" customHeight="1"/>
-    <row r="354" ht="14.25" customHeight="1"/>
-    <row r="355" ht="14.25" customHeight="1"/>
-    <row r="356" ht="14.25" customHeight="1"/>
-    <row r="357" ht="14.25" customHeight="1"/>
-    <row r="358" ht="14.25" customHeight="1"/>
-    <row r="359" ht="14.25" customHeight="1"/>
-    <row r="360" ht="14.25" customHeight="1"/>
-    <row r="361" ht="14.25" customHeight="1"/>
-    <row r="362" ht="14.25" customHeight="1"/>
-    <row r="363" ht="14.25" customHeight="1"/>
-    <row r="364" ht="14.25" customHeight="1"/>
-    <row r="365" ht="14.25" customHeight="1"/>
-    <row r="366" ht="14.25" customHeight="1"/>
-    <row r="367" ht="14.25" customHeight="1"/>
-    <row r="368" ht="14.25" customHeight="1"/>
-    <row r="369" ht="14.25" customHeight="1"/>
-    <row r="370" ht="14.25" customHeight="1"/>
-    <row r="371" ht="14.25" customHeight="1"/>
-    <row r="372" ht="14.25" customHeight="1"/>
-    <row r="373" ht="14.25" customHeight="1"/>
-    <row r="374" ht="14.25" customHeight="1"/>
-    <row r="375" ht="14.25" customHeight="1"/>
-    <row r="376" ht="14.25" customHeight="1"/>
-    <row r="377" ht="14.25" customHeight="1"/>
-    <row r="378" ht="14.25" customHeight="1"/>
-    <row r="379" ht="14.25" customHeight="1"/>
-    <row r="380" ht="14.25" customHeight="1"/>
-    <row r="381" ht="14.25" customHeight="1"/>
-    <row r="382" ht="14.25" customHeight="1"/>
-    <row r="383" ht="14.25" customHeight="1"/>
-    <row r="384" ht="14.25" customHeight="1"/>
-    <row r="385" ht="14.25" customHeight="1"/>
-    <row r="386" ht="14.25" customHeight="1"/>
-    <row r="387" ht="14.25" customHeight="1"/>
-    <row r="388" ht="14.25" customHeight="1"/>
-    <row r="389" ht="14.25" customHeight="1"/>
-    <row r="390" ht="14.25" customHeight="1"/>
-    <row r="391" ht="14.25" customHeight="1"/>
-    <row r="392" ht="14.25" customHeight="1"/>
-    <row r="393" ht="14.25" customHeight="1"/>
-    <row r="394" ht="14.25" customHeight="1"/>
-    <row r="395" ht="14.25" customHeight="1"/>
-    <row r="396" ht="14.25" customHeight="1"/>
-    <row r="397" ht="14.25" customHeight="1"/>
-    <row r="398" ht="14.25" customHeight="1"/>
-    <row r="399" ht="14.25" customHeight="1"/>
-    <row r="400" ht="14.25" customHeight="1"/>
-    <row r="401" ht="14.25" customHeight="1"/>
-    <row r="402" ht="14.25" customHeight="1"/>
-    <row r="403" ht="14.25" customHeight="1"/>
-    <row r="404" ht="14.25" customHeight="1"/>
-    <row r="405" ht="14.25" customHeight="1"/>
-    <row r="406" ht="14.25" customHeight="1"/>
-    <row r="407" ht="14.25" customHeight="1"/>
-    <row r="408" ht="14.25" customHeight="1"/>
-    <row r="409" ht="14.25" customHeight="1"/>
-    <row r="410" ht="14.25" customHeight="1"/>
-    <row r="411" ht="14.25" customHeight="1"/>
-    <row r="412" ht="14.25" customHeight="1"/>
-    <row r="413" ht="14.25" customHeight="1"/>
-    <row r="414" ht="14.25" customHeight="1"/>
-    <row r="415" ht="14.25" customHeight="1"/>
-    <row r="416" ht="14.25" customHeight="1"/>
-    <row r="417" ht="14.25" customHeight="1"/>
-    <row r="418" ht="14.25" customHeight="1"/>
-    <row r="419" ht="14.25" customHeight="1"/>
-    <row r="420" ht="14.25" customHeight="1"/>
-    <row r="421" ht="14.25" customHeight="1"/>
-    <row r="422" ht="14.25" customHeight="1"/>
-    <row r="423" ht="14.25" customHeight="1"/>
-    <row r="424" ht="14.25" customHeight="1"/>
-    <row r="425" ht="14.25" customHeight="1"/>
-    <row r="426" ht="14.25" customHeight="1"/>
-    <row r="427" ht="14.25" customHeight="1"/>
-    <row r="428" ht="14.25" customHeight="1"/>
-    <row r="429" ht="14.25" customHeight="1"/>
-    <row r="430" ht="14.25" customHeight="1"/>
-    <row r="431" ht="14.25" customHeight="1"/>
-    <row r="432" ht="14.25" customHeight="1"/>
-    <row r="433" ht="14.25" customHeight="1"/>
-    <row r="434" ht="14.25" customHeight="1"/>
-    <row r="435" ht="14.25" customHeight="1"/>
-    <row r="436" ht="14.25" customHeight="1"/>
-    <row r="437" ht="14.25" customHeight="1"/>
-    <row r="438" ht="14.25" customHeight="1"/>
-    <row r="439" ht="14.25" customHeight="1"/>
-    <row r="440" ht="14.25" customHeight="1"/>
-    <row r="441" ht="14.25" customHeight="1"/>
-    <row r="442" ht="14.25" customHeight="1"/>
-    <row r="443" ht="14.25" customHeight="1"/>
-    <row r="444" ht="14.25" customHeight="1"/>
-    <row r="445" ht="14.25" customHeight="1"/>
-    <row r="446" ht="14.25" customHeight="1"/>
-    <row r="447" ht="14.25" customHeight="1"/>
-    <row r="448" ht="14.25" customHeight="1"/>
-    <row r="449" ht="14.25" customHeight="1"/>
-    <row r="450" ht="14.25" customHeight="1"/>
-    <row r="451" ht="14.25" customHeight="1"/>
-    <row r="452" ht="14.25" customHeight="1"/>
-    <row r="453" ht="14.25" customHeight="1"/>
-    <row r="454" ht="14.25" customHeight="1"/>
-    <row r="455" ht="14.25" customHeight="1"/>
-    <row r="456" ht="14.25" customHeight="1"/>
-    <row r="457" ht="14.25" customHeight="1"/>
-    <row r="458" ht="14.25" customHeight="1"/>
-    <row r="459" ht="14.25" customHeight="1"/>
-    <row r="460" ht="14.25" customHeight="1"/>
-    <row r="461" ht="14.25" customHeight="1"/>
-    <row r="462" ht="14.25" customHeight="1"/>
-    <row r="463" ht="14.25" customHeight="1"/>
-    <row r="464" ht="14.25" customHeight="1"/>
-    <row r="465" ht="14.25" customHeight="1"/>
-    <row r="466" ht="14.25" customHeight="1"/>
-    <row r="467" ht="14.25" customHeight="1"/>
-    <row r="468" ht="14.25" customHeight="1"/>
-    <row r="469" ht="14.25" customHeight="1"/>
-    <row r="470" ht="14.25" customHeight="1"/>
-    <row r="471" ht="14.25" customHeight="1"/>
-    <row r="472" ht="14.25" customHeight="1"/>
-    <row r="473" ht="14.25" customHeight="1"/>
-    <row r="474" ht="14.25" customHeight="1"/>
-    <row r="475" ht="14.25" customHeight="1"/>
-    <row r="476" ht="14.25" customHeight="1"/>
-    <row r="477" ht="14.25" customHeight="1"/>
-    <row r="478" ht="14.25" customHeight="1"/>
-    <row r="479" ht="14.25" customHeight="1"/>
-    <row r="480" ht="14.25" customHeight="1"/>
-    <row r="481" ht="14.25" customHeight="1"/>
-    <row r="482" ht="14.25" customHeight="1"/>
-    <row r="483" ht="14.25" customHeight="1"/>
-    <row r="484" ht="14.25" customHeight="1"/>
-    <row r="485" ht="14.25" customHeight="1"/>
-    <row r="486" ht="14.25" customHeight="1"/>
-    <row r="487" ht="14.25" customHeight="1"/>
-    <row r="488" ht="14.25" customHeight="1"/>
-    <row r="489" ht="14.25" customHeight="1"/>
-    <row r="490" ht="14.25" customHeight="1"/>
-    <row r="491" ht="14.25" customHeight="1"/>
-    <row r="492" ht="14.25" customHeight="1"/>
-    <row r="493" ht="14.25" customHeight="1"/>
-    <row r="494" ht="14.25" customHeight="1"/>
-    <row r="495" ht="14.25" customHeight="1"/>
-    <row r="496" ht="14.25" customHeight="1"/>
-    <row r="497" ht="14.25" customHeight="1"/>
-    <row r="498" ht="14.25" customHeight="1"/>
-    <row r="499" ht="14.25" customHeight="1"/>
-    <row r="500" ht="14.25" customHeight="1"/>
-    <row r="501" ht="14.25" customHeight="1"/>
-    <row r="502" ht="14.25" customHeight="1"/>
-    <row r="503" ht="14.25" customHeight="1"/>
-    <row r="504" ht="14.25" customHeight="1"/>
-    <row r="505" ht="14.25" customHeight="1"/>
-    <row r="506" ht="14.25" customHeight="1"/>
-    <row r="507" ht="14.25" customHeight="1"/>
-    <row r="508" ht="14.25" customHeight="1"/>
-    <row r="509" ht="14.25" customHeight="1"/>
-    <row r="510" ht="14.25" customHeight="1"/>
-    <row r="511" ht="14.25" customHeight="1"/>
-    <row r="512" ht="14.25" customHeight="1"/>
-    <row r="513" ht="14.25" customHeight="1"/>
-    <row r="514" ht="14.25" customHeight="1"/>
-    <row r="515" ht="14.25" customHeight="1"/>
-    <row r="516" ht="14.25" customHeight="1"/>
-    <row r="517" ht="14.25" customHeight="1"/>
-    <row r="518" ht="14.25" customHeight="1"/>
-    <row r="519" ht="14.25" customHeight="1"/>
-    <row r="520" ht="14.25" customHeight="1"/>
-    <row r="521" ht="14.25" customHeight="1"/>
-    <row r="522" ht="14.25" customHeight="1"/>
-    <row r="523" ht="14.25" customHeight="1"/>
-    <row r="524" ht="14.25" customHeight="1"/>
-    <row r="525" ht="14.25" customHeight="1"/>
-    <row r="526" ht="14.25" customHeight="1"/>
-    <row r="527" ht="14.25" customHeight="1"/>
-    <row r="528" ht="14.25" customHeight="1"/>
-    <row r="529" ht="14.25" customHeight="1"/>
-    <row r="530" ht="14.25" customHeight="1"/>
-    <row r="531" ht="14.25" customHeight="1"/>
-    <row r="532" ht="14.25" customHeight="1"/>
-    <row r="533" ht="14.25" customHeight="1"/>
-    <row r="534" ht="14.25" customHeight="1"/>
-    <row r="535" ht="14.25" customHeight="1"/>
-    <row r="536" ht="14.25" customHeight="1"/>
-    <row r="537" ht="14.25" customHeight="1"/>
-    <row r="538" ht="14.25" customHeight="1"/>
-    <row r="539" ht="14.25" customHeight="1"/>
-    <row r="540" ht="14.25" customHeight="1"/>
-    <row r="541" ht="14.25" customHeight="1"/>
-    <row r="542" ht="14.25" customHeight="1"/>
-    <row r="543" ht="14.25" customHeight="1"/>
-    <row r="544" ht="14.25" customHeight="1"/>
-    <row r="545" ht="14.25" customHeight="1"/>
-    <row r="546" ht="14.25" customHeight="1"/>
-    <row r="547" ht="14.25" customHeight="1"/>
-    <row r="548" ht="14.25" customHeight="1"/>
-    <row r="549" ht="14.25" customHeight="1"/>
-    <row r="550" ht="14.25" customHeight="1"/>
-    <row r="551" ht="14.25" customHeight="1"/>
-    <row r="552" ht="14.25" customHeight="1"/>
-    <row r="553" ht="14.25" customHeight="1"/>
-    <row r="554" ht="14.25" customHeight="1"/>
-    <row r="555" ht="14.25" customHeight="1"/>
-    <row r="556" ht="14.25" customHeight="1"/>
-    <row r="557" ht="14.25" customHeight="1"/>
-    <row r="558" ht="14.25" customHeight="1"/>
-    <row r="559" ht="14.25" customHeight="1"/>
-    <row r="560" ht="14.25" customHeight="1"/>
-    <row r="561" ht="14.25" customHeight="1"/>
-    <row r="562" ht="14.25" customHeight="1"/>
-    <row r="563" ht="14.25" customHeight="1"/>
-    <row r="564" ht="14.25" customHeight="1"/>
-    <row r="565" ht="14.25" customHeight="1"/>
-    <row r="566" ht="14.25" customHeight="1"/>
-    <row r="567" ht="14.25" customHeight="1"/>
-    <row r="568" ht="14.25" customHeight="1"/>
-    <row r="569" ht="14.25" customHeight="1"/>
-    <row r="570" ht="14.25" customHeight="1"/>
-    <row r="571" ht="14.25" customHeight="1"/>
-    <row r="572" ht="14.25" customHeight="1"/>
-    <row r="573" ht="14.25" customHeight="1"/>
-    <row r="574" ht="14.25" customHeight="1"/>
-    <row r="575" ht="14.25" customHeight="1"/>
-    <row r="576" ht="14.25" customHeight="1"/>
-    <row r="577" ht="14.25" customHeight="1"/>
-    <row r="578" ht="14.25" customHeight="1"/>
-    <row r="579" ht="14.25" customHeight="1"/>
-    <row r="580" ht="14.25" customHeight="1"/>
-    <row r="581" ht="14.25" customHeight="1"/>
-    <row r="582" ht="14.25" customHeight="1"/>
-    <row r="583" ht="14.25" customHeight="1"/>
-    <row r="584" ht="14.25" customHeight="1"/>
-    <row r="585" ht="14.25" customHeight="1"/>
-    <row r="586" ht="14.25" customHeight="1"/>
-    <row r="587" ht="14.25" customHeight="1"/>
-    <row r="588" ht="14.25" customHeight="1"/>
-    <row r="589" ht="14.25" customHeight="1"/>
-    <row r="590" ht="14.25" customHeight="1"/>
-    <row r="591" ht="14.25" customHeight="1"/>
-    <row r="592" ht="14.25" customHeight="1"/>
-    <row r="593" ht="14.25" customHeight="1"/>
-    <row r="594" ht="14.25" customHeight="1"/>
-    <row r="595" ht="14.25" customHeight="1"/>
-    <row r="596" ht="14.25" customHeight="1"/>
-    <row r="597" ht="14.25" customHeight="1"/>
-    <row r="598" ht="14.25" customHeight="1"/>
-    <row r="599" ht="14.25" customHeight="1"/>
-    <row r="600" ht="14.25" customHeight="1"/>
-    <row r="601" ht="14.25" customHeight="1"/>
-    <row r="602" ht="14.25" customHeight="1"/>
-    <row r="603" ht="14.25" customHeight="1"/>
-    <row r="604" ht="14.25" customHeight="1"/>
-    <row r="605" ht="14.25" customHeight="1"/>
-    <row r="606" ht="14.25" customHeight="1"/>
-    <row r="607" ht="14.25" customHeight="1"/>
-    <row r="608" ht="14.25" customHeight="1"/>
-    <row r="609" ht="14.25" customHeight="1"/>
-    <row r="610" ht="14.25" customHeight="1"/>
-    <row r="611" ht="14.25" customHeight="1"/>
-    <row r="612" ht="14.25" customHeight="1"/>
-    <row r="613" ht="14.25" customHeight="1"/>
-    <row r="614" ht="14.25" customHeight="1"/>
-    <row r="615" ht="14.25" customHeight="1"/>
-    <row r="616" ht="14.25" customHeight="1"/>
-    <row r="617" ht="14.25" customHeight="1"/>
-    <row r="618" ht="14.25" customHeight="1"/>
-    <row r="619" ht="14.25" customHeight="1"/>
-    <row r="620" ht="14.25" customHeight="1"/>
-    <row r="621" ht="14.25" customHeight="1"/>
-    <row r="622" ht="14.25" customHeight="1"/>
-    <row r="623" ht="14.25" customHeight="1"/>
-    <row r="624" ht="14.25" customHeight="1"/>
-    <row r="625" ht="14.25" customHeight="1"/>
-    <row r="626" ht="14.25" customHeight="1"/>
-    <row r="627" ht="14.25" customHeight="1"/>
-    <row r="628" ht="14.25" customHeight="1"/>
-    <row r="629" ht="14.25" customHeight="1"/>
-    <row r="630" ht="14.25" customHeight="1"/>
-    <row r="631" ht="14.25" customHeight="1"/>
-    <row r="632" ht="14.25" customHeight="1"/>
-    <row r="633" ht="14.25" customHeight="1"/>
-    <row r="634" ht="14.25" customHeight="1"/>
-    <row r="635" ht="14.25" customHeight="1"/>
-    <row r="636" ht="14.25" customHeight="1"/>
-    <row r="637" ht="14.25" customHeight="1"/>
-    <row r="638" ht="14.25" customHeight="1"/>
-    <row r="639" ht="14.25" customHeight="1"/>
-    <row r="640" ht="14.25" customHeight="1"/>
-    <row r="641" ht="14.25" customHeight="1"/>
-    <row r="642" ht="14.25" customHeight="1"/>
-    <row r="643" ht="14.25" customHeight="1"/>
-    <row r="644" ht="14.25" customHeight="1"/>
-    <row r="645" ht="14.25" customHeight="1"/>
-    <row r="646" ht="14.25" customHeight="1"/>
-    <row r="647" ht="14.25" customHeight="1"/>
-    <row r="648" ht="14.25" customHeight="1"/>
-    <row r="649" ht="14.25" customHeight="1"/>
-    <row r="650" ht="14.25" customHeight="1"/>
-    <row r="651" ht="14.25" customHeight="1"/>
-    <row r="652" ht="14.25" customHeight="1"/>
-    <row r="653" ht="14.25" customHeight="1"/>
-    <row r="654" ht="14.25" customHeight="1"/>
-    <row r="655" ht="14.25" customHeight="1"/>
-    <row r="656" ht="14.25" customHeight="1"/>
-    <row r="657" ht="14.25" customHeight="1"/>
-    <row r="658" ht="14.25" customHeight="1"/>
-    <row r="659" ht="14.25" customHeight="1"/>
-    <row r="660" ht="14.25" customHeight="1"/>
-    <row r="661" ht="14.25" customHeight="1"/>
-    <row r="662" ht="14.25" customHeight="1"/>
-    <row r="663" ht="14.25" customHeight="1"/>
-    <row r="664" ht="14.25" customHeight="1"/>
-    <row r="665" ht="14.25" customHeight="1"/>
-    <row r="666" ht="14.25" customHeight="1"/>
-    <row r="667" ht="14.25" customHeight="1"/>
-    <row r="668" ht="14.25" customHeight="1"/>
-    <row r="669" ht="14.25" customHeight="1"/>
-    <row r="670" ht="14.25" customHeight="1"/>
-    <row r="671" ht="14.25" customHeight="1"/>
-    <row r="672" ht="14.25" customHeight="1"/>
-    <row r="673" ht="14.25" customHeight="1"/>
-    <row r="674" ht="14.25" customHeight="1"/>
-    <row r="675" ht="14.25" customHeight="1"/>
-    <row r="676" ht="14.25" customHeight="1"/>
-    <row r="677" ht="14.25" customHeight="1"/>
-    <row r="678" ht="14.25" customHeight="1"/>
-    <row r="679" ht="14.25" customHeight="1"/>
-    <row r="680" ht="14.25" customHeight="1"/>
-    <row r="681" ht="14.25" customHeight="1"/>
-    <row r="682" ht="14.25" customHeight="1"/>
-    <row r="683" ht="14.25" customHeight="1"/>
-    <row r="684" ht="14.25" customHeight="1"/>
-    <row r="685" ht="14.25" customHeight="1"/>
-    <row r="686" ht="14.25" customHeight="1"/>
-    <row r="687" ht="14.25" customHeight="1"/>
-    <row r="688" ht="14.25" customHeight="1"/>
-    <row r="689" ht="14.25" customHeight="1"/>
-    <row r="690" ht="14.25" customHeight="1"/>
-    <row r="691" ht="14.25" customHeight="1"/>
-    <row r="692" ht="14.25" customHeight="1"/>
-    <row r="693" ht="14.25" customHeight="1"/>
-    <row r="694" ht="14.25" customHeight="1"/>
-    <row r="695" ht="14.25" customHeight="1"/>
-    <row r="696" ht="14.25" customHeight="1"/>
-    <row r="697" ht="14.25" customHeight="1"/>
-    <row r="698" ht="14.25" customHeight="1"/>
-    <row r="699" ht="14.25" customHeight="1"/>
-    <row r="700" ht="14.25" customHeight="1"/>
-    <row r="701" ht="14.25" customHeight="1"/>
-    <row r="702" ht="14.25" customHeight="1"/>
-    <row r="703" ht="14.25" customHeight="1"/>
-    <row r="704" ht="14.25" customHeight="1"/>
-    <row r="705" ht="14.25" customHeight="1"/>
-    <row r="706" ht="14.25" customHeight="1"/>
-    <row r="707" ht="14.25" customHeight="1"/>
-    <row r="708" ht="14.25" customHeight="1"/>
-    <row r="709" ht="14.25" customHeight="1"/>
-    <row r="710" ht="14.25" customHeight="1"/>
-    <row r="711" ht="14.25" customHeight="1"/>
-    <row r="712" ht="14.25" customHeight="1"/>
-    <row r="713" ht="14.25" customHeight="1"/>
-    <row r="714" ht="14.25" customHeight="1"/>
-    <row r="715" ht="14.25" customHeight="1"/>
-    <row r="716" ht="14.25" customHeight="1"/>
-    <row r="717" ht="14.25" customHeight="1"/>
-    <row r="718" ht="14.25" customHeight="1"/>
-    <row r="719" ht="14.25" customHeight="1"/>
-    <row r="720" ht="14.25" customHeight="1"/>
-    <row r="721" ht="14.25" customHeight="1"/>
-    <row r="722" ht="14.25" customHeight="1"/>
-    <row r="723" ht="14.25" customHeight="1"/>
-    <row r="724" ht="14.25" customHeight="1"/>
-    <row r="725" ht="14.25" customHeight="1"/>
-    <row r="726" ht="14.25" customHeight="1"/>
-    <row r="727" ht="14.25" customHeight="1"/>
-    <row r="728" ht="14.25" customHeight="1"/>
-    <row r="729" ht="14.25" customHeight="1"/>
-    <row r="730" ht="14.25" customHeight="1"/>
-    <row r="731" ht="14.25" customHeight="1"/>
-    <row r="732" ht="14.25" customHeight="1"/>
-    <row r="733" ht="14.25" customHeight="1"/>
-    <row r="734" ht="14.25" customHeight="1"/>
-    <row r="735" ht="14.25" customHeight="1"/>
-    <row r="736" ht="14.25" customHeight="1"/>
-    <row r="737" ht="14.25" customHeight="1"/>
-    <row r="738" ht="14.25" customHeight="1"/>
-    <row r="739" ht="14.25" customHeight="1"/>
-    <row r="740" ht="14.25" customHeight="1"/>
-    <row r="741" ht="14.25" customHeight="1"/>
-    <row r="742" ht="14.25" customHeight="1"/>
-    <row r="743" ht="14.25" customHeight="1"/>
-    <row r="744" ht="14.25" customHeight="1"/>
-    <row r="745" ht="14.25" customHeight="1"/>
-    <row r="746" ht="14.25" customHeight="1"/>
-    <row r="747" ht="14.25" customHeight="1"/>
-    <row r="748" ht="14.25" customHeight="1"/>
-    <row r="749" ht="14.25" customHeight="1"/>
-    <row r="750" ht="14.25" customHeight="1"/>
-    <row r="751" ht="14.25" customHeight="1"/>
-    <row r="752" ht="14.25" customHeight="1"/>
-    <row r="753" ht="14.25" customHeight="1"/>
-    <row r="754" ht="14.25" customHeight="1"/>
-    <row r="755" ht="14.25" customHeight="1"/>
-    <row r="756" ht="14.25" customHeight="1"/>
-    <row r="757" ht="14.25" customHeight="1"/>
-    <row r="758" ht="14.25" customHeight="1"/>
-    <row r="759" ht="14.25" customHeight="1"/>
-    <row r="760" ht="14.25" customHeight="1"/>
-    <row r="761" ht="14.25" customHeight="1"/>
-    <row r="762" ht="14.25" customHeight="1"/>
-    <row r="763" ht="14.25" customHeight="1"/>
-    <row r="764" ht="14.25" customHeight="1"/>
-    <row r="765" ht="14.25" customHeight="1"/>
-    <row r="766" ht="14.25" customHeight="1"/>
-    <row r="767" ht="14.25" customHeight="1"/>
-    <row r="768" ht="14.25" customHeight="1"/>
-    <row r="769" ht="14.25" customHeight="1"/>
-    <row r="770" ht="14.25" customHeight="1"/>
-    <row r="771" ht="14.25" customHeight="1"/>
-    <row r="772" ht="14.25" customHeight="1"/>
-    <row r="773" ht="14.25" customHeight="1"/>
-    <row r="774" ht="14.25" customHeight="1"/>
-    <row r="775" ht="14.25" customHeight="1"/>
-    <row r="776" ht="14.25" customHeight="1"/>
-    <row r="777" ht="14.25" customHeight="1"/>
-    <row r="778" ht="14.25" customHeight="1"/>
-    <row r="779" ht="14.25" customHeight="1"/>
-    <row r="780" ht="14.25" customHeight="1"/>
-    <row r="781" ht="14.25" customHeight="1"/>
-    <row r="782" ht="14.25" customHeight="1"/>
-    <row r="783" ht="14.25" customHeight="1"/>
-    <row r="784" ht="14.25" customHeight="1"/>
-    <row r="785" ht="14.25" customHeight="1"/>
-    <row r="786" ht="14.25" customHeight="1"/>
-    <row r="787" ht="14.25" customHeight="1"/>
-    <row r="788" ht="14.25" customHeight="1"/>
-    <row r="789" ht="14.25" customHeight="1"/>
-    <row r="790" ht="14.25" customHeight="1"/>
-    <row r="791" ht="14.25" customHeight="1"/>
-    <row r="792" ht="14.25" customHeight="1"/>
-    <row r="793" ht="14.25" customHeight="1"/>
-    <row r="794" ht="14.25" customHeight="1"/>
-    <row r="795" ht="14.25" customHeight="1"/>
-    <row r="796" ht="14.25" customHeight="1"/>
-    <row r="797" ht="14.25" customHeight="1"/>
-    <row r="798" ht="14.25" customHeight="1"/>
-    <row r="799" ht="14.25" customHeight="1"/>
-    <row r="800" ht="14.25" customHeight="1"/>
-    <row r="801" ht="14.25" customHeight="1"/>
-    <row r="802" ht="14.25" customHeight="1"/>
-    <row r="803" ht="14.25" customHeight="1"/>
-    <row r="804" ht="14.25" customHeight="1"/>
-    <row r="805" ht="14.25" customHeight="1"/>
-    <row r="806" ht="14.25" customHeight="1"/>
-    <row r="807" ht="14.25" customHeight="1"/>
-    <row r="808" ht="14.25" customHeight="1"/>
-    <row r="809" ht="14.25" customHeight="1"/>
-    <row r="810" ht="14.25" customHeight="1"/>
-    <row r="811" ht="14.25" customHeight="1"/>
-    <row r="812" ht="14.25" customHeight="1"/>
-    <row r="813" ht="14.25" customHeight="1"/>
-    <row r="814" ht="14.25" customHeight="1"/>
-    <row r="815" ht="14.25" customHeight="1"/>
-    <row r="816" ht="14.25" customHeight="1"/>
-    <row r="817" ht="14.25" customHeight="1"/>
-    <row r="818" ht="14.25" customHeight="1"/>
-    <row r="819" ht="14.25" customHeight="1"/>
-    <row r="820" ht="14.25" customHeight="1"/>
-    <row r="821" ht="14.25" customHeight="1"/>
-    <row r="822" ht="14.25" customHeight="1"/>
-    <row r="823" ht="14.25" customHeight="1"/>
-    <row r="824" ht="14.25" customHeight="1"/>
-    <row r="825" ht="14.25" customHeight="1"/>
-    <row r="826" ht="14.25" customHeight="1"/>
-    <row r="827" ht="14.25" customHeight="1"/>
-    <row r="828" ht="14.25" customHeight="1"/>
-    <row r="829" ht="14.25" customHeight="1"/>
-    <row r="830" ht="14.25" customHeight="1"/>
-    <row r="831" ht="14.25" customHeight="1"/>
-    <row r="832" ht="14.25" customHeight="1"/>
-    <row r="833" ht="14.25" customHeight="1"/>
-    <row r="834" ht="14.25" customHeight="1"/>
-    <row r="835" ht="14.25" customHeight="1"/>
-    <row r="836" ht="14.25" customHeight="1"/>
-    <row r="837" ht="14.25" customHeight="1"/>
-    <row r="838" ht="14.25" customHeight="1"/>
-    <row r="839" ht="14.25" customHeight="1"/>
-    <row r="840" ht="14.25" customHeight="1"/>
-    <row r="841" ht="14.25" customHeight="1"/>
-    <row r="842" ht="14.25" customHeight="1"/>
-    <row r="843" ht="14.25" customHeight="1"/>
-    <row r="844" ht="14.25" customHeight="1"/>
-    <row r="845" ht="14.25" customHeight="1"/>
-    <row r="846" ht="14.25" customHeight="1"/>
-    <row r="847" ht="14.25" customHeight="1"/>
-    <row r="848" ht="14.25" customHeight="1"/>
-    <row r="849" ht="14.25" customHeight="1"/>
-    <row r="850" ht="14.25" customHeight="1"/>
-    <row r="851" ht="14.25" customHeight="1"/>
-    <row r="852" ht="14.25" customHeight="1"/>
-    <row r="853" ht="14.25" customHeight="1"/>
-    <row r="854" ht="14.25" customHeight="1"/>
-    <row r="855" ht="14.25" customHeight="1"/>
-    <row r="856" ht="14.25" customHeight="1"/>
-    <row r="857" ht="14.25" customHeight="1"/>
-    <row r="858" ht="14.25" customHeight="1"/>
-    <row r="859" ht="14.25" customHeight="1"/>
-    <row r="860" ht="14.25" customHeight="1"/>
-    <row r="861" ht="14.25" customHeight="1"/>
-    <row r="862" ht="14.25" customHeight="1"/>
-    <row r="863" ht="14.25" customHeight="1"/>
-    <row r="864" ht="14.25" customHeight="1"/>
-    <row r="865" ht="14.25" customHeight="1"/>
-    <row r="866" ht="14.25" customHeight="1"/>
-    <row r="867" ht="14.25" customHeight="1"/>
-    <row r="868" ht="14.25" customHeight="1"/>
-    <row r="869" ht="14.25" customHeight="1"/>
-    <row r="870" ht="14.25" customHeight="1"/>
-    <row r="871" ht="14.25" customHeight="1"/>
-    <row r="872" ht="14.25" customHeight="1"/>
-    <row r="873" ht="14.25" customHeight="1"/>
-    <row r="874" ht="14.25" customHeight="1"/>
-    <row r="875" ht="14.25" customHeight="1"/>
-    <row r="876" ht="14.25" customHeight="1"/>
-    <row r="877" ht="14.25" customHeight="1"/>
-    <row r="878" ht="14.25" customHeight="1"/>
-    <row r="879" ht="14.25" customHeight="1"/>
-    <row r="880" ht="14.25" customHeight="1"/>
-    <row r="881" ht="14.25" customHeight="1"/>
-    <row r="882" ht="14.25" customHeight="1"/>
-    <row r="883" ht="14.25" customHeight="1"/>
-    <row r="884" ht="14.25" customHeight="1"/>
-    <row r="885" ht="14.25" customHeight="1"/>
-    <row r="886" ht="14.25" customHeight="1"/>
-    <row r="887" ht="14.25" customHeight="1"/>
-    <row r="888" ht="14.25" customHeight="1"/>
-    <row r="889" ht="14.25" customHeight="1"/>
-    <row r="890" ht="14.25" customHeight="1"/>
-    <row r="891" ht="14.25" customHeight="1"/>
-    <row r="892" ht="14.25" customHeight="1"/>
-    <row r="893" ht="14.25" customHeight="1"/>
-    <row r="894" ht="14.25" customHeight="1"/>
-    <row r="895" ht="14.25" customHeight="1"/>
-    <row r="896" ht="14.25" customHeight="1"/>
-    <row r="897" ht="14.25" customHeight="1"/>
-    <row r="898" ht="14.25" customHeight="1"/>
-    <row r="899" ht="14.25" customHeight="1"/>
-    <row r="900" ht="14.25" customHeight="1"/>
-    <row r="901" ht="14.25" customHeight="1"/>
-    <row r="902" ht="14.25" customHeight="1"/>
-    <row r="903" ht="14.25" customHeight="1"/>
-    <row r="904" ht="14.25" customHeight="1"/>
-    <row r="905" ht="14.25" customHeight="1"/>
-    <row r="906" ht="14.25" customHeight="1"/>
-    <row r="907" ht="14.25" customHeight="1"/>
-    <row r="908" ht="14.25" customHeight="1"/>
-    <row r="909" ht="14.25" customHeight="1"/>
-    <row r="910" ht="14.25" customHeight="1"/>
-    <row r="911" ht="14.25" customHeight="1"/>
-    <row r="912" ht="14.25" customHeight="1"/>
-    <row r="913" ht="14.25" customHeight="1"/>
-    <row r="914" ht="14.25" customHeight="1"/>
-    <row r="915" ht="14.25" customHeight="1"/>
-    <row r="916" ht="14.25" customHeight="1"/>
-    <row r="917" ht="14.25" customHeight="1"/>
-    <row r="918" ht="14.25" customHeight="1"/>
-    <row r="919" ht="14.25" customHeight="1"/>
-    <row r="920" ht="14.25" customHeight="1"/>
-    <row r="921" ht="14.25" customHeight="1"/>
-    <row r="922" ht="14.25" customHeight="1"/>
-    <row r="923" ht="14.25" customHeight="1"/>
-    <row r="924" ht="14.25" customHeight="1"/>
-    <row r="925" ht="14.25" customHeight="1"/>
-    <row r="926" ht="14.25" customHeight="1"/>
-    <row r="927" ht="14.25" customHeight="1"/>
-    <row r="928" ht="14.25" customHeight="1"/>
-    <row r="929" ht="14.25" customHeight="1"/>
-    <row r="930" ht="14.25" customHeight="1"/>
-    <row r="931" ht="14.25" customHeight="1"/>
-    <row r="932" ht="14.25" customHeight="1"/>
-    <row r="933" ht="14.25" customHeight="1"/>
-    <row r="934" ht="14.25" customHeight="1"/>
-    <row r="935" ht="14.25" customHeight="1"/>
-    <row r="936" ht="14.25" customHeight="1"/>
-    <row r="937" ht="14.25" customHeight="1"/>
-    <row r="938" ht="14.25" customHeight="1"/>
-    <row r="939" ht="14.25" customHeight="1"/>
-    <row r="940" ht="14.25" customHeight="1"/>
-    <row r="941" ht="14.25" customHeight="1"/>
-    <row r="942" ht="14.25" customHeight="1"/>
-    <row r="943" ht="14.25" customHeight="1"/>
-    <row r="944" ht="14.25" customHeight="1"/>
-    <row r="945" ht="14.25" customHeight="1"/>
-    <row r="946" ht="14.25" customHeight="1"/>
-    <row r="947" ht="14.25" customHeight="1"/>
-    <row r="948" ht="14.25" customHeight="1"/>
-    <row r="949" ht="14.25" customHeight="1"/>
-    <row r="950" ht="14.25" customHeight="1"/>
-    <row r="951" ht="14.25" customHeight="1"/>
-    <row r="952" ht="14.25" customHeight="1"/>
-    <row r="953" ht="14.25" customHeight="1"/>
-    <row r="954" ht="14.25" customHeight="1"/>
-    <row r="955" ht="14.25" customHeight="1"/>
-    <row r="956" ht="14.25" customHeight="1"/>
-    <row r="957" ht="14.25" customHeight="1"/>
-    <row r="958" ht="14.25" customHeight="1"/>
-    <row r="959" ht="14.25" customHeight="1"/>
-    <row r="960" ht="14.25" customHeight="1"/>
-    <row r="961" ht="14.25" customHeight="1"/>
-    <row r="962" ht="14.25" customHeight="1"/>
-    <row r="963" ht="14.25" customHeight="1"/>
-    <row r="964" ht="14.25" customHeight="1"/>
-    <row r="965" ht="14.25" customHeight="1"/>
-    <row r="966" ht="14.25" customHeight="1"/>
-    <row r="967" ht="14.25" customHeight="1"/>
-    <row r="968" ht="14.25" customHeight="1"/>
-    <row r="969" ht="14.25" customHeight="1"/>
-    <row r="970" ht="14.25" customHeight="1"/>
-    <row r="971" ht="14.25" customHeight="1"/>
-    <row r="972" ht="14.25" customHeight="1"/>
-    <row r="973" ht="14.25" customHeight="1"/>
-    <row r="974" ht="14.25" customHeight="1"/>
-    <row r="975" ht="14.25" customHeight="1"/>
-    <row r="976" ht="14.25" customHeight="1"/>
-    <row r="977" ht="14.25" customHeight="1"/>
-    <row r="978" ht="14.25" customHeight="1"/>
-    <row r="979" ht="14.25" customHeight="1"/>
-    <row r="980" ht="14.25" customHeight="1"/>
-    <row r="981" ht="14.25" customHeight="1"/>
-    <row r="982" ht="14.25" customHeight="1"/>
-    <row r="983" ht="14.25" customHeight="1"/>
-    <row r="984" ht="14.25" customHeight="1"/>
-    <row r="985" ht="14.25" customHeight="1"/>
-    <row r="986" ht="14.25" customHeight="1"/>
-    <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
-    <row r="989" ht="14.25" customHeight="1"/>
-    <row r="990" ht="14.25" customHeight="1"/>
-    <row r="991" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:38" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="89" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="92" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="97" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="98" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="99" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="100" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="101" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="102" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="103" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="104" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="105" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="106" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="107" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="108" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="109" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="110" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="111" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="112" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="113" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="114" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="115" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="116" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="117" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="118" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="119" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="120" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="121" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="122" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="123" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="124" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="125" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="126" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="127" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="128" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="129" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="130" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="131" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="132" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="133" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="134" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="135" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="136" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="137" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="138" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="139" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="140" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="141" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="142" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="143" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="144" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="145" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="146" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="147" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="148" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="149" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="150" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="151" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="152" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="153" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="154" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="155" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="156" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="157" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="158" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="159" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="160" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="161" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="163" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="164" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="165" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="167" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="168" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="169" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="170" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="171" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="172" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="173" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="174" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="175" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="176" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="177" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="178" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="179" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="180" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="181" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="182" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="183" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="184" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="185" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="186" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="187" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="188" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="189" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="190" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="191" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="192" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="193" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="194" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="195" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="196" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="197" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="198" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="199" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="200" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="201" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="202" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="203" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="204" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="205" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="206" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="207" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="208" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="209" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="210" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="211" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="212" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="213" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="214" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="215" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="216" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="217" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="218" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="219" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="220" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="221" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="222" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="223" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="224" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="225" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="226" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="227" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="228" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="229" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="230" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="231" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="232" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="233" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="234" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="235" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="236" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="237" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="238" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="239" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="240" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="241" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="242" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="243" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="244" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="245" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="246" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="247" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="248" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="249" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="250" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="251" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="252" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="253" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="254" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="255" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="256" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="257" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="258" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="259" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="260" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="261" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="262" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="263" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="264" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="265" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="266" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="267" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="268" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="269" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="270" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="271" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="272" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="273" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="274" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="275" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="276" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="277" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="278" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="279" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="280" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="281" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="282" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="283" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="284" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="285" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="286" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="287" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="288" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="289" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="290" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="291" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="292" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="293" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="294" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="295" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="296" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="297" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="298" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="299" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="300" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="301" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="302" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="303" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="304" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="305" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="306" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="307" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="308" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="309" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="310" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="311" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="312" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="313" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="314" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="315" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="316" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="317" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="318" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="319" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="320" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="321" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="322" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="323" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="324" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="325" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="326" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="327" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="328" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="329" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="330" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="331" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="332" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="333" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="334" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="335" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="336" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="337" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="338" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="339" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="340" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="341" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="342" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="343" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="344" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="345" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="346" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="347" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="348" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="349" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="350" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="351" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="352" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="353" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="354" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="355" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="356" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="357" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="358" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="359" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="360" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="361" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="362" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="363" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="364" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="365" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="366" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="367" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="368" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="369" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="370" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="371" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="372" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="373" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="374" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="375" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="376" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="377" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="378" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="379" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="380" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="381" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="382" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="383" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="384" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="385" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="386" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="387" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="388" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="389" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="390" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="391" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="392" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="393" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="394" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="395" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="396" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="397" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="398" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="399" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="400" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="401" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="402" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="403" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="404" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="405" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="406" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="407" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="408" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="409" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="410" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="411" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="412" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="413" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="414" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="415" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="416" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="417" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="418" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="419" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="420" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="421" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="422" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="423" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="424" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="425" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="426" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="427" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="428" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="429" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="430" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="431" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="432" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="433" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="434" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="435" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="436" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="437" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="438" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="439" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="440" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="441" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="442" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="443" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="444" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="445" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="446" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="447" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="448" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="449" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="450" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="451" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="452" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="453" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="454" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="455" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="456" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="457" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="458" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="459" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="460" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="461" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="462" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="463" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="464" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="465" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="466" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="467" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="468" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="469" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="470" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="471" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="472" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="473" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="474" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="475" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="476" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="477" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="478" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="479" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="480" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="481" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="482" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="483" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="484" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="485" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="486" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="487" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="488" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="489" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="490" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="491" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="492" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="493" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="494" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="495" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="496" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="497" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="498" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="499" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="500" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="501" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="502" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="503" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="504" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="505" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="506" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="507" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="508" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="509" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="510" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="511" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="512" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="513" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="514" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="515" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="516" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="517" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="518" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="519" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="520" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="521" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="522" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="523" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="524" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="525" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="526" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="527" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="528" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="529" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="530" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="531" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="532" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="533" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="534" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="535" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="536" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="537" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="538" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="539" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="540" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="541" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="542" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="543" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="544" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="545" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="546" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="547" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="548" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="549" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="550" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="551" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="552" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="553" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="554" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="555" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="556" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="557" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="558" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="559" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="560" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="561" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="562" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="563" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="564" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="565" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="566" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="567" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="568" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="569" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="570" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="571" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="572" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="573" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="574" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="575" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="576" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="577" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="578" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="579" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="580" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="581" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="582" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="583" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="584" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="585" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="586" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="587" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="588" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="589" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="590" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="591" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="592" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="593" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="594" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="595" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="596" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="597" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="598" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="599" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="600" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="601" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="602" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="603" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="604" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="605" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="606" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="607" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="608" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="609" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="610" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="611" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="612" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="613" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="614" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="615" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="616" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="617" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="618" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="619" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="620" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="621" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="622" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="623" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="624" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="625" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="626" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="627" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="628" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="629" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="630" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="631" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="632" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="633" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="634" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="635" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="636" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="637" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="638" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="639" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="640" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="641" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="642" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="643" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="644" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="645" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="646" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="647" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="648" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="649" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="650" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="651" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="652" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="653" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="654" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="655" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="656" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="657" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="658" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="659" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="660" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="661" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="662" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="663" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="664" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="665" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="666" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="667" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="668" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="669" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="670" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="671" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="672" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="673" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="674" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="675" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="676" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="677" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="678" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="679" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="680" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="681" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="682" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="683" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="684" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="685" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="686" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="687" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="688" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="689" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="690" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="691" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="692" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="693" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="694" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="695" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="696" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="697" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="698" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="699" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="700" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="701" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="702" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="703" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="704" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="705" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="706" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="707" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="708" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="709" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="710" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="711" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="712" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="713" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="714" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="715" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="716" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="717" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="718" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="719" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="720" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="721" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="722" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="723" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="724" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="725" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="726" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="727" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="728" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="729" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="730" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="731" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="732" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="733" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="734" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="735" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="736" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="737" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="738" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="739" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="740" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="741" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="742" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="743" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="744" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="745" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="746" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="747" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="748" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="749" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="750" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="751" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="752" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="753" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="754" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="755" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="756" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="757" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="758" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="759" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="760" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="761" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="762" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="763" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="764" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="765" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="766" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="767" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="768" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="769" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="770" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="771" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="772" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="773" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="774" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="775" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="776" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="777" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="778" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="779" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="780" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="781" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="782" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="783" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="784" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="785" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="786" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="787" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="788" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="789" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="790" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="791" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="792" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="793" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="794" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="795" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="796" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="797" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="798" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="799" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="800" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="801" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="802" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="803" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="804" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="805" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="806" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="807" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="808" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="809" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="810" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="811" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="812" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="813" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="814" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="815" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="816" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="817" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="818" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="819" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="820" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="821" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="822" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="823" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="824" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="825" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="826" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="827" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="828" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="829" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="830" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="831" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="832" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="833" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="834" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="835" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="836" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="837" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="838" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="839" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="840" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="841" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="842" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="843" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="844" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="845" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="846" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="847" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="848" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="849" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="850" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="851" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="852" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="853" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="854" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="855" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="856" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="857" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="858" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="859" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="860" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="861" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="862" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="863" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="864" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="865" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="866" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="867" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="868" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="869" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="870" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="871" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="872" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="873" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="874" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="875" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="876" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="877" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="878" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="879" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="880" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="881" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="882" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="883" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="884" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="885" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="886" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="887" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="888" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="889" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="890" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="891" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="892" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="893" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="894" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="895" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="896" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="897" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="898" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="899" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="900" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="901" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="902" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="903" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="904" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="905" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="906" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="907" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="908" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="909" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="910" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="911" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="912" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="913" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="914" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="915" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="916" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="917" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="918" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="919" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="920" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="921" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="922" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="923" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="924" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="925" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="926" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="927" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="928" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="929" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="930" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="931" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="932" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="933" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="934" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="935" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="936" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="937" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="938" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="939" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="940" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="941" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="942" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="943" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="944" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="945" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="946" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="947" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="948" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="949" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="950" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="951" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="952" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="953" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="954" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="955" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="956" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="957" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="958" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="959" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="960" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="961" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="962" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="963" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="964" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="965" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="966" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="967" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="968" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="969" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="970" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="971" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="972" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="973" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="974" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="975" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="976" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="977" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="978" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="979" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="980" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="981" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="982" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="E1:AH5"/>
@@ -4824,13 +5288,13 @@
     <mergeCell ref="E26:AH26"/>
   </mergeCells>
   <conditionalFormatting sqref="E10:AH23">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"E"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"A"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4850,6 +5314,496 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{108E628D-0699-DF48-9B99-F1B00778B412}">
+  <dimension ref="A2:B61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" s="25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" s="10"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" s="10"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" s="10"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47" s="10"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48" s="10"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B49" s="10"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B50" s="10"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B51" s="10"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B52" s="10"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B53" s="10"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B54" s="10"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B55" s="10"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B56" s="10"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B57" s="10"/>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B58" s="10"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B59" s="10"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B60" s="10"/>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B61" s="10"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:B31">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>"E"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>"P"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+      <formula>"A"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32:B61">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"E"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"P"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"A"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B22:B23 B26:B31 B44:B61" xr:uid="{1C0BFE0E-5C0A-EA44-9705-E025C1AD6291}">
+      <formula1>"P,E,A,០,L"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4860,6 +5814,16 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6d203857-9991-4518-a1a2-8110fc6be8da">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F0858A9B289063469BE04336DE235773" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5a2df236b8c77d00588fa208ad4b3c13">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6d203857-9991-4518-a1a2-8110fc6be8da" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2b600674eb87e46e051f2a311ef7ec87" ns2:_="">
     <xsd:import namespace="6d203857-9991-4518-a1a2-8110fc6be8da"/>
@@ -5031,24 +5995,38 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6d203857-9991-4518-a1a2-8110fc6be8da">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E327CF2-7FDD-4039-AC38-602BCD2BAA13}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E327CF2-7FDD-4039-AC38-602BCD2BAA13}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00A8542F-4870-469B-BC0F-A7A36A618599}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{367249C4-D492-4CC0-8B9A-6C97B063DE02}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6d203857-9991-4518-a1a2-8110fc6be8da"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{367249C4-D492-4CC0-8B9A-6C97B063DE02}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00A8542F-4870-469B-BC0F-A7A36A618599}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6d203857-9991-4518-a1a2-8110fc6be8da"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>